<commit_message>
docs warehouse customer emoployee
</commit_message>
<xml_diff>
--- a/docs/documentacao.xlsx
+++ b/docs/documentacao.xlsx
@@ -5,20 +5,23 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micaelmbp/Documents/ENG-2022/TAAD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micaelmbp/Documents/ENG-2022/TAAD/GlobalTech_ETL/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7FDF71-1BEE-A249-B021-743D95EEE1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832CAC64-A47C-BE49-A3F4-9149CBCDF043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="1900" windowWidth="46080" windowHeight="25480" activeTab="1" xr2:uid="{1C0ABE59-C842-1448-8BFE-1E96A6C9A910}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="3" xr2:uid="{1C0ABE59-C842-1448-8BFE-1E96A6C9A910}"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz de decisão" sheetId="1" r:id="rId1"/>
-    <sheet name="Caracterização da dimensão  (2)" sheetId="7" r:id="rId2"/>
-    <sheet name="Caracterização da dimensão X" sheetId="4" r:id="rId3"/>
-    <sheet name="Caracterização da TF X" sheetId="3" r:id="rId4"/>
-    <sheet name="Metadata" sheetId="5" r:id="rId5"/>
-    <sheet name="Change Log" sheetId="6" r:id="rId6"/>
+    <sheet name="DIM Warehouse" sheetId="7" r:id="rId2"/>
+    <sheet name="DIM Employee" sheetId="9" r:id="rId3"/>
+    <sheet name="DIM Customer" sheetId="4" r:id="rId4"/>
+    <sheet name="DIM Order" sheetId="8" r:id="rId5"/>
+    <sheet name="TF Order Payment" sheetId="11" r:id="rId6"/>
+    <sheet name="TF Order" sheetId="3" r:id="rId7"/>
+    <sheet name="Metadata" sheetId="5" r:id="rId8"/>
+    <sheet name="Change Log" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="115">
   <si>
     <t>Caracterização do Data Mart</t>
   </si>
@@ -320,6 +323,69 @@
   </si>
   <si>
     <t>region</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>South San Francisco</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>Americas</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Funcionários da empresa</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>hire_date</t>
+  </si>
+  <si>
+    <t>Quem é o seu superior</t>
+  </si>
+  <si>
+    <t>Tommy</t>
+  </si>
+  <si>
+    <t>Bailey</t>
+  </si>
+  <si>
+    <t>2016-06-17 00:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>city -&gt; state -&gt; country -&gt; region</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>Clientes que realizam as encomendas</t>
   </si>
 </sst>
 </file>
@@ -984,16 +1050,67 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1014,55 +1131,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1074,40 +1173,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7193,8 +7259,8 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7204,93 +7270,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="93"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="85"/>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="86" t="s">
         <v>88</v>
       </c>
       <c r="C2" s="60"/>
       <c r="D2" s="60"/>
       <c r="E2" s="60"/>
       <c r="F2" s="60"/>
-      <c r="G2" s="68"/>
+      <c r="G2" s="87"/>
     </row>
     <row r="3" spans="1:7" ht="46" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="72" t="s">
         <v>89</v>
       </c>
       <c r="C3" s="61"/>
       <c r="D3" s="61"/>
       <c r="E3" s="61"/>
       <c r="F3" s="61"/>
-      <c r="G3" s="70"/>
+      <c r="G3" s="73"/>
     </row>
     <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="72" t="s">
         <v>52</v>
       </c>
       <c r="C4" s="61"/>
       <c r="D4" s="61"/>
       <c r="E4" s="61"/>
       <c r="F4" s="61"/>
-      <c r="G4" s="70"/>
+      <c r="G4" s="73"/>
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="69"/>
+      <c r="B5" s="72" t="s">
+        <v>88</v>
+      </c>
       <c r="C5" s="61"/>
       <c r="D5" s="61"/>
       <c r="E5" s="61"/>
       <c r="F5" s="61"/>
-      <c r="G5" s="70"/>
+      <c r="G5" s="73"/>
     </row>
     <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="71"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="74" t="s">
+      <c r="B6" s="88"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="75"/>
-      <c r="G6" s="76"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="93"/>
     </row>
     <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="35"/>
       <c r="G7" s="33"/>
     </row>
     <row r="8" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="88" t="s">
+      <c r="A8" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="89"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="90"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="82"/>
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
@@ -7320,61 +7388,95 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -7510,9 +7612,15 @@
       <c r="G27" s="79"/>
     </row>
     <row r="28" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="66"/>
+      <c r="A28" s="1">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="66" t="s">
+        <v>111</v>
+      </c>
       <c r="D28" s="66"/>
       <c r="E28" s="66"/>
       <c r="F28" s="66"/>
@@ -7541,7 +7649,7 @@
       <c r="G31" s="33"/>
     </row>
     <row r="32" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="86" t="s">
+      <c r="A32" s="67" t="s">
         <v>22</v>
       </c>
       <c r="B32" s="63"/>
@@ -7549,28 +7657,28 @@
       <c r="D32" s="63"/>
       <c r="E32" s="63"/>
       <c r="F32" s="63"/>
-      <c r="G32" s="87"/>
+      <c r="G32" s="68"/>
     </row>
     <row r="33" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="80"/>
-      <c r="B33" s="81"/>
-      <c r="C33" s="81"/>
-      <c r="D33" s="81"/>
-      <c r="E33" s="81"/>
-      <c r="F33" s="81"/>
-      <c r="G33" s="82"/>
+      <c r="A33" s="69"/>
+      <c r="B33" s="70"/>
+      <c r="C33" s="70"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="70"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="71"/>
     </row>
     <row r="34" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="80"/>
-      <c r="B34" s="81"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="81"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="81"/>
-      <c r="G34" s="82"/>
+      <c r="A34" s="69"/>
+      <c r="B34" s="70"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="71"/>
     </row>
     <row r="35" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="86" t="s">
+      <c r="A35" s="67" t="s">
         <v>10</v>
       </c>
       <c r="B35" s="63"/>
@@ -7578,38 +7686,35 @@
       <c r="D35" s="63"/>
       <c r="E35" s="63"/>
       <c r="F35" s="63"/>
-      <c r="G35" s="87"/>
+      <c r="G35" s="68"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="69"/>
+      <c r="A36" s="72"/>
       <c r="B36" s="61"/>
       <c r="C36" s="61"/>
       <c r="D36" s="61"/>
       <c r="E36" s="61"/>
       <c r="F36" s="61"/>
-      <c r="G36" s="70"/>
+      <c r="G36" s="73"/>
     </row>
     <row r="37" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="83"/>
-      <c r="B37" s="84"/>
-      <c r="C37" s="84"/>
-      <c r="D37" s="84"/>
-      <c r="E37" s="84"/>
-      <c r="F37" s="84"/>
-      <c r="G37" s="85"/>
+      <c r="A37" s="74"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A33:G34"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A36:G37"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="A18:G18"/>
@@ -7617,13 +7722,16 @@
     <mergeCell ref="D20:G20"/>
     <mergeCell ref="D21:G21"/>
     <mergeCell ref="D22:G22"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A33:G34"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A36:G37"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Exemplo:_x000a_id -&gt; nome -&gt; categoria -&gt; ALL" sqref="C28:C31" xr:uid="{386320E1-7050-C749-9143-6F7D856CB823}"/>
@@ -7666,7 +7774,7 @@
           <x14:formula1>
             <xm:f>Metadata!$A$15:$A$17</xm:f>
           </x14:formula1>
-          <xm:sqref>B4 F10</xm:sqref>
+          <xm:sqref>B4 F10:F14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -7675,14 +7783,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08161B19-BCEA-2046-88B5-D5F1C39CCC68}">
-  <sheetPr codeName="Sheet3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689679D6-004F-8547-939A-39369E55E211}">
+  <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7692,85 +7800,607 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="93"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="85"/>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="67"/>
+      <c r="B2" s="86" t="s">
+        <v>100</v>
+      </c>
       <c r="C2" s="60"/>
       <c r="D2" s="60"/>
       <c r="E2" s="60"/>
       <c r="F2" s="60"/>
-      <c r="G2" s="68"/>
+      <c r="G2" s="87"/>
     </row>
     <row r="3" spans="1:7" ht="46" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="69"/>
+      <c r="B3" s="72" t="s">
+        <v>101</v>
+      </c>
       <c r="C3" s="61"/>
       <c r="D3" s="61"/>
       <c r="E3" s="61"/>
       <c r="F3" s="61"/>
-      <c r="G3" s="70"/>
+      <c r="G3" s="73"/>
     </row>
     <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="69"/>
+      <c r="B4" s="72" t="s">
+        <v>54</v>
+      </c>
       <c r="C4" s="61"/>
       <c r="D4" s="61"/>
       <c r="E4" s="61"/>
       <c r="F4" s="61"/>
-      <c r="G4" s="70"/>
+      <c r="G4" s="73"/>
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="69"/>
+      <c r="B5" s="72" t="s">
+        <v>100</v>
+      </c>
       <c r="C5" s="61"/>
       <c r="D5" s="61"/>
       <c r="E5" s="61"/>
       <c r="F5" s="61"/>
-      <c r="G5" s="70"/>
+      <c r="G5" s="73"/>
     </row>
     <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="71"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="76"/>
+      <c r="B6" s="88"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="92"/>
+      <c r="G6" s="93"/>
     </row>
     <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="35"/>
       <c r="G7" s="33"/>
     </row>
     <row r="8" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="88" t="s">
+      <c r="A8" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="89"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="90"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="82"/>
+    </row>
+    <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="36"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="37"/>
+    </row>
+    <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="78" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="56"/>
+    </row>
+    <row r="19" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="79" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="79"/>
+    </row>
+    <row r="20" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="77"/>
+    </row>
+    <row r="21" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="77"/>
+    </row>
+    <row r="22" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="77"/>
+    </row>
+    <row r="23" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="77"/>
+      <c r="G23" s="77"/>
+    </row>
+    <row r="24" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="77"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="77"/>
+      <c r="G24" s="77"/>
+    </row>
+    <row r="25" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A25" s="36"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="29"/>
+      <c r="G25" s="33"/>
+    </row>
+    <row r="26" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A26" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="55"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="56"/>
+    </row>
+    <row r="27" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A27" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="79" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="79"/>
+    </row>
+    <row r="28" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+    </row>
+    <row r="29" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="66"/>
+    </row>
+    <row r="30" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+    </row>
+    <row r="31" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="G31" s="33"/>
+    </row>
+    <row r="32" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="68"/>
+    </row>
+    <row r="33" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="69"/>
+      <c r="B33" s="70"/>
+      <c r="C33" s="70"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="70"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="71"/>
+    </row>
+    <row r="34" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="69"/>
+      <c r="B34" s="70"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="71"/>
+    </row>
+    <row r="35" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="63"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="68"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="72"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="61"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="73"/>
+    </row>
+    <row r="37" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="74"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="76"/>
+    </row>
+  </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A33:G34"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A36:G37"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+  </mergeCells>
+  <dataValidations count="4">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Colocar percentagem" sqref="B6" xr:uid="{F51EFD33-359E-334A-A51E-A657A56E6972}">
+      <formula1>1</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Posição do atributo na tabela (posição ordinal)" sqref="A10:A17" xr:uid="{89530213-4BB8-BA43-9CD1-9672B684A608}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Identificação" sqref="A20" xr:uid="{6EBC917B-F748-9D47-AC30-86DD4039D676}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Exemplo:_x000a_id -&gt; nome -&gt; categoria -&gt; ALL" sqref="C28:C31" xr:uid="{DCD299E7-07EE-0E44-A747-001C4034EE3C}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{55EC4112-973B-FC4C-A084-8465525BE94F}">
+          <x14:formula1>
+            <xm:f>Metadata!$A$15:$A$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>B4 F10:F13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2C02D4C8-5807-1B42-A575-AD6C9C5C405A}">
+          <x14:formula1>
+            <xm:f>Metadata!$A$27:$A$29</xm:f>
+          </x14:formula1>
+          <xm:sqref>D10:D17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E6A9F69E-8530-554F-84ED-06A617D22C16}">
+          <x14:formula1>
+            <xm:f>Metadata!$A$33:$A$34</xm:f>
+          </x14:formula1>
+          <xm:sqref>C20</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B58DB043-F4BA-0B4A-8912-6E90381FA2F8}">
+          <x14:formula1>
+            <xm:f>Metadata!$A$37:$A$41</xm:f>
+          </x14:formula1>
+          <xm:sqref>D20:D25</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Etiqueta temporal_x000a_" xr:uid="{2FF847AC-2296-2A4D-99F0-730709725FC8}">
+          <x14:formula1>
+            <xm:f>Metadata!$A$21:$A$23</xm:f>
+          </x14:formula1>
+          <xm:sqref>E6:G6</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08161B19-BCEA-2046-88B5-D5F1C39CCC68}">
+  <sheetPr codeName="Sheet3">
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.1640625" customWidth="1"/>
+    <col min="2" max="7" width="30.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="83" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="85"/>
+    </row>
+    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="86" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="87"/>
+    </row>
+    <row r="3" spans="1:7" ht="46" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="73"/>
+    </row>
+    <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="72"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="73"/>
+    </row>
+    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="72" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="73"/>
+    </row>
+    <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="88"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="93"/>
+    </row>
+    <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="35"/>
+      <c r="G7" s="33"/>
+    </row>
+    <row r="8" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="80" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="82"/>
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
@@ -8005,7 +8635,7 @@
       <c r="G31" s="33"/>
     </row>
     <row r="32" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="86" t="s">
+      <c r="A32" s="67" t="s">
         <v>22</v>
       </c>
       <c r="B32" s="63"/>
@@ -8013,28 +8643,28 @@
       <c r="D32" s="63"/>
       <c r="E32" s="63"/>
       <c r="F32" s="63"/>
-      <c r="G32" s="87"/>
+      <c r="G32" s="68"/>
     </row>
     <row r="33" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="80"/>
-      <c r="B33" s="81"/>
-      <c r="C33" s="81"/>
-      <c r="D33" s="81"/>
-      <c r="E33" s="81"/>
-      <c r="F33" s="81"/>
-      <c r="G33" s="82"/>
+      <c r="A33" s="69"/>
+      <c r="B33" s="70"/>
+      <c r="C33" s="70"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="70"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="71"/>
     </row>
     <row r="34" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="80"/>
-      <c r="B34" s="81"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="81"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="81"/>
-      <c r="G34" s="82"/>
+      <c r="A34" s="69"/>
+      <c r="B34" s="70"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="71"/>
     </row>
     <row r="35" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="86" t="s">
+      <c r="A35" s="67" t="s">
         <v>10</v>
       </c>
       <c r="B35" s="63"/>
@@ -8042,28 +8672,36 @@
       <c r="D35" s="63"/>
       <c r="E35" s="63"/>
       <c r="F35" s="63"/>
-      <c r="G35" s="87"/>
+      <c r="G35" s="68"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="69"/>
+      <c r="A36" s="72"/>
       <c r="B36" s="61"/>
       <c r="C36" s="61"/>
       <c r="D36" s="61"/>
       <c r="E36" s="61"/>
       <c r="F36" s="61"/>
-      <c r="G36" s="70"/>
+      <c r="G36" s="73"/>
     </row>
     <row r="37" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="83"/>
-      <c r="B37" s="84"/>
-      <c r="C37" s="84"/>
-      <c r="D37" s="84"/>
-      <c r="E37" s="84"/>
-      <c r="F37" s="84"/>
-      <c r="G37" s="85"/>
+      <c r="A37" s="74"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D23:G23"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="D20:G20"/>
@@ -8080,14 +8718,6 @@
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="C27:G27"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Colocar percentagem" sqref="B6" xr:uid="{C5DD908A-3688-A14E-B89F-E074FAFCDF99}">
@@ -8138,15 +8768,479 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45AE6A66-6571-D24D-A307-DF57ADB3F673}">
-  <sheetPr codeName="Sheet4">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{008ECA3F-6D43-6440-9C18-66C320EDE763}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.1640625" customWidth="1"/>
+    <col min="2" max="7" width="30.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="83" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="85"/>
+    </row>
+    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="86"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="87"/>
+    </row>
+    <row r="3" spans="1:7" ht="46" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="72"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="73"/>
+    </row>
+    <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="72"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="73"/>
+    </row>
+    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="72"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="73"/>
+    </row>
+    <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="88"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="93"/>
+    </row>
+    <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="35"/>
+      <c r="G7" s="33"/>
+    </row>
+    <row r="8" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="80" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="82"/>
+    </row>
+    <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="36"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="37"/>
+    </row>
+    <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="78" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="56"/>
+    </row>
+    <row r="19" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="79" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="79"/>
+    </row>
+    <row r="20" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="77"/>
+    </row>
+    <row r="21" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="77"/>
+    </row>
+    <row r="22" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="77"/>
+    </row>
+    <row r="23" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="77"/>
+      <c r="G23" s="77"/>
+    </row>
+    <row r="24" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="77"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="77"/>
+      <c r="G24" s="77"/>
+    </row>
+    <row r="25" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A25" s="36"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="29"/>
+      <c r="G25" s="33"/>
+    </row>
+    <row r="26" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A26" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="55"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="56"/>
+    </row>
+    <row r="27" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A27" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="79" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="79"/>
+    </row>
+    <row r="28" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+    </row>
+    <row r="29" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="66"/>
+    </row>
+    <row r="30" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+    </row>
+    <row r="31" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="G31" s="33"/>
+    </row>
+    <row r="32" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="68"/>
+    </row>
+    <row r="33" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="69"/>
+      <c r="B33" s="70"/>
+      <c r="C33" s="70"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="70"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="71"/>
+    </row>
+    <row r="34" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="69"/>
+      <c r="B34" s="70"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="71"/>
+    </row>
+    <row r="35" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="63"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="68"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="72"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="61"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="73"/>
+    </row>
+    <row r="37" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="74"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="76"/>
+    </row>
+  </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A33:G34"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A36:G37"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+  </mergeCells>
+  <dataValidations count="4">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Exemplo:_x000a_id -&gt; nome -&gt; categoria -&gt; ALL" sqref="C28:C31" xr:uid="{6749BA4D-A4C0-664A-8057-C07B807E371B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Identificação" sqref="A20" xr:uid="{931E409E-69F5-FE4E-AEB1-ADDD7B40042D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Posição do atributo na tabela (posição ordinal)" sqref="A10:A17" xr:uid="{C40D2E8E-CF02-1E46-B718-7497F7BB1DE6}"/>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Colocar percentagem" sqref="B6" xr:uid="{C62A5CB1-E417-6D44-BE27-17DBBADE6A9F}">
+      <formula1>1</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Etiqueta temporal_x000a_" xr:uid="{D5194091-E172-7B4B-93F1-B350A039B133}">
+          <x14:formula1>
+            <xm:f>Metadata!$A$21:$A$23</xm:f>
+          </x14:formula1>
+          <xm:sqref>E6:G6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4E10733A-5A8E-6743-BD42-25CA375F0172}">
+          <x14:formula1>
+            <xm:f>Metadata!$A$37:$A$41</xm:f>
+          </x14:formula1>
+          <xm:sqref>D20:D25</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D0857C76-E4C6-9648-B76B-1341A72605EF}">
+          <x14:formula1>
+            <xm:f>Metadata!$A$33:$A$34</xm:f>
+          </x14:formula1>
+          <xm:sqref>C20</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{96B37CFB-0B55-DA48-908F-7A932548E70A}">
+          <x14:formula1>
+            <xm:f>Metadata!$A$27:$A$29</xm:f>
+          </x14:formula1>
+          <xm:sqref>D10:D17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{697E1F21-4492-A949-842D-03E00B0BFFFE}">
+          <x14:formula1>
+            <xm:f>Metadata!$A$15:$A$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>B4 F10</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0538C7DA-5E49-754B-91B9-6A82D176845B}">
+  <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8155,132 +9249,132 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="83" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="93"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="85"/>
     </row>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="99"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="97"/>
     </row>
     <row r="3" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="101"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="102"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="99"/>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="101"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="102"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="99"/>
     </row>
     <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="101"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="102"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="99"/>
     </row>
     <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="101"/>
-      <c r="C6" s="101"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="102"/>
+      <c r="B6" s="98"/>
+      <c r="C6" s="98"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="99"/>
     </row>
     <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="101"/>
-      <c r="C7" s="101"/>
-      <c r="D7" s="101"/>
-      <c r="E7" s="101"/>
-      <c r="F7" s="102"/>
+      <c r="B7" s="98"/>
+      <c r="C7" s="98"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="99"/>
     </row>
     <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="101"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="102"/>
+      <c r="B8" s="98"/>
+      <c r="C8" s="98"/>
+      <c r="D8" s="98"/>
+      <c r="E8" s="98"/>
+      <c r="F8" s="99"/>
     </row>
     <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="101"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="102"/>
+      <c r="B9" s="98"/>
+      <c r="C9" s="98"/>
+      <c r="D9" s="98"/>
+      <c r="E9" s="98"/>
+      <c r="F9" s="99"/>
     </row>
     <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="102"/>
+      <c r="B10" s="98"/>
+      <c r="C10" s="98"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="98"/>
+      <c r="F10" s="99"/>
     </row>
     <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="104"/>
-      <c r="C11" s="104"/>
-      <c r="D11" s="104"/>
-      <c r="E11" s="104"/>
-      <c r="F11" s="105"/>
+      <c r="B11" s="94"/>
+      <c r="C11" s="94"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="95"/>
     </row>
     <row r="12" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="94"/>
-      <c r="B12" s="95"/>
-      <c r="C12" s="95"/>
-      <c r="D12" s="95"/>
-      <c r="E12" s="95"/>
-      <c r="F12" s="96"/>
+      <c r="A12" s="105"/>
+      <c r="B12" s="106"/>
+      <c r="C12" s="106"/>
+      <c r="D12" s="106"/>
+      <c r="E12" s="106"/>
+      <c r="F12" s="107"/>
     </row>
     <row r="13" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="88" t="s">
+      <c r="A13" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="89"/>
-      <c r="C13" s="89"/>
-      <c r="D13" s="89"/>
-      <c r="E13" s="89"/>
-      <c r="F13" s="90"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="82"/>
     </row>
     <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
@@ -8359,22 +9453,22 @@
       <c r="F21" s="43"/>
     </row>
     <row r="22" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="94"/>
-      <c r="B22" s="95"/>
-      <c r="C22" s="95"/>
-      <c r="D22" s="95"/>
-      <c r="E22" s="95"/>
-      <c r="F22" s="96"/>
+      <c r="A22" s="105"/>
+      <c r="B22" s="106"/>
+      <c r="C22" s="106"/>
+      <c r="D22" s="106"/>
+      <c r="E22" s="106"/>
+      <c r="F22" s="107"/>
     </row>
     <row r="23" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="88" t="s">
+      <c r="A23" s="80" t="s">
         <v>78</v>
       </c>
-      <c r="B23" s="89"/>
-      <c r="C23" s="89"/>
-      <c r="D23" s="89"/>
-      <c r="E23" s="89"/>
-      <c r="F23" s="90"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="82"/>
     </row>
     <row r="24" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="39" t="s">
@@ -8429,22 +9523,22 @@
       <c r="F28" s="43"/>
     </row>
     <row r="29" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="94"/>
-      <c r="B29" s="95"/>
-      <c r="C29" s="95"/>
-      <c r="D29" s="95"/>
-      <c r="E29" s="95"/>
-      <c r="F29" s="96"/>
+      <c r="A29" s="105"/>
+      <c r="B29" s="106"/>
+      <c r="C29" s="106"/>
+      <c r="D29" s="106"/>
+      <c r="E29" s="106"/>
+      <c r="F29" s="107"/>
     </row>
     <row r="30" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="88" t="s">
+      <c r="A30" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="89"/>
-      <c r="C30" s="89"/>
-      <c r="D30" s="89"/>
-      <c r="E30" s="89"/>
-      <c r="F30" s="90"/>
+      <c r="B30" s="81"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="81"/>
+      <c r="F30" s="82"/>
     </row>
     <row r="31" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="39" t="s">
@@ -8456,114 +9550,648 @@
       <c r="C31" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="98" t="s">
+      <c r="D31" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="98"/>
-      <c r="F31" s="99"/>
+      <c r="E31" s="96"/>
+      <c r="F31" s="97"/>
     </row>
     <row r="32" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="39"/>
       <c r="B32" s="40"/>
       <c r="C32" s="40"/>
-      <c r="D32" s="101"/>
-      <c r="E32" s="101"/>
-      <c r="F32" s="102"/>
+      <c r="D32" s="98"/>
+      <c r="E32" s="98"/>
+      <c r="F32" s="99"/>
     </row>
     <row r="33" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="39"/>
       <c r="B33" s="40"/>
       <c r="C33" s="40"/>
-      <c r="D33" s="101"/>
-      <c r="E33" s="101"/>
-      <c r="F33" s="102"/>
+      <c r="D33" s="98"/>
+      <c r="E33" s="98"/>
+      <c r="F33" s="99"/>
     </row>
     <row r="34" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="39"/>
       <c r="B34" s="40"/>
       <c r="C34" s="40"/>
-      <c r="D34" s="101"/>
-      <c r="E34" s="101"/>
-      <c r="F34" s="102"/>
+      <c r="D34" s="98"/>
+      <c r="E34" s="98"/>
+      <c r="F34" s="99"/>
     </row>
     <row r="35" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="41"/>
       <c r="B35" s="42"/>
       <c r="C35" s="42"/>
-      <c r="D35" s="104"/>
-      <c r="E35" s="104"/>
-      <c r="F35" s="105"/>
+      <c r="D35" s="94"/>
+      <c r="E35" s="94"/>
+      <c r="F35" s="95"/>
     </row>
     <row r="36" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="106"/>
-      <c r="B36" s="107"/>
-      <c r="C36" s="107"/>
-      <c r="D36" s="107"/>
-      <c r="E36" s="107"/>
-      <c r="F36" s="108"/>
+      <c r="A36" s="102"/>
+      <c r="B36" s="103"/>
+      <c r="C36" s="103"/>
+      <c r="D36" s="103"/>
+      <c r="E36" s="103"/>
+      <c r="F36" s="104"/>
     </row>
     <row r="37" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="88" t="s">
+      <c r="A37" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="89"/>
-      <c r="C37" s="89"/>
-      <c r="D37" s="89"/>
-      <c r="E37" s="89"/>
-      <c r="F37" s="90"/>
+      <c r="B37" s="81"/>
+      <c r="C37" s="81"/>
+      <c r="D37" s="81"/>
+      <c r="E37" s="81"/>
+      <c r="F37" s="82"/>
     </row>
     <row r="38" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="97"/>
-      <c r="B38" s="98"/>
-      <c r="C38" s="98"/>
-      <c r="D38" s="98"/>
-      <c r="E38" s="98"/>
-      <c r="F38" s="99"/>
+      <c r="A38" s="100"/>
+      <c r="B38" s="96"/>
+      <c r="C38" s="96"/>
+      <c r="D38" s="96"/>
+      <c r="E38" s="96"/>
+      <c r="F38" s="97"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="100"/>
-      <c r="B39" s="101"/>
-      <c r="C39" s="101"/>
-      <c r="D39" s="101"/>
-      <c r="E39" s="101"/>
-      <c r="F39" s="102"/>
+      <c r="A39" s="108"/>
+      <c r="B39" s="98"/>
+      <c r="C39" s="98"/>
+      <c r="D39" s="98"/>
+      <c r="E39" s="98"/>
+      <c r="F39" s="99"/>
     </row>
     <row r="40" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="94"/>
-      <c r="B40" s="95"/>
-      <c r="C40" s="95"/>
-      <c r="D40" s="95"/>
-      <c r="E40" s="95"/>
-      <c r="F40" s="96"/>
+      <c r="A40" s="105"/>
+      <c r="B40" s="106"/>
+      <c r="C40" s="106"/>
+      <c r="D40" s="106"/>
+      <c r="E40" s="106"/>
+      <c r="F40" s="107"/>
     </row>
     <row r="41" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="88" t="s">
+      <c r="A41" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="B41" s="89"/>
-      <c r="C41" s="89"/>
-      <c r="D41" s="89"/>
-      <c r="E41" s="89"/>
-      <c r="F41" s="90"/>
+      <c r="B41" s="81"/>
+      <c r="C41" s="81"/>
+      <c r="D41" s="81"/>
+      <c r="E41" s="81"/>
+      <c r="F41" s="82"/>
     </row>
     <row r="42" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="97"/>
-      <c r="B42" s="98"/>
-      <c r="C42" s="98"/>
-      <c r="D42" s="98"/>
-      <c r="E42" s="98"/>
-      <c r="F42" s="99"/>
+      <c r="A42" s="100"/>
+      <c r="B42" s="96"/>
+      <c r="C42" s="96"/>
+      <c r="D42" s="96"/>
+      <c r="E42" s="96"/>
+      <c r="F42" s="97"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="103"/>
-      <c r="B43" s="104"/>
-      <c r="C43" s="104"/>
-      <c r="D43" s="104"/>
-      <c r="E43" s="104"/>
-      <c r="F43" s="105"/>
+      <c r="A43" s="101"/>
+      <c r="B43" s="94"/>
+      <c r="C43" s="94"/>
+      <c r="D43" s="94"/>
+      <c r="E43" s="94"/>
+      <c r="F43" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A38:F39"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A42:F43"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+  </mergeCells>
+  <dataValidations count="5">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Exemplo:_x000a_&quot;Dados dos últimos 4 anos&quot;" sqref="B11:F11" xr:uid="{ABE851E0-8AAB-564B-9AA0-54BD36B0E9AB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Exemplo:_x000a_&quot;Entre as 2 e as 5 da manhã&quot;" sqref="B8:F8" xr:uid="{09D39043-6DF2-AC4D-BC84-2F2B67EE89CD}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Exemplo:_x000a_&quot;Incentivar as vendas de telemóveis&quot;" sqref="B6:F6" xr:uid="{AE6422FE-C2E3-2940-B39D-4D219ECB59A7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nome do data mart ao qual a tabela de factos pertence" sqref="B4:F4" xr:uid="{6FCADBAD-5161-5549-A93E-131F4AD7AFDF}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Colocar percentagem_x000a_" sqref="B10:C10" xr:uid="{C64D4F59-7D3D-EB4D-90A8-BB9417FB3DF0}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3C4ACE68-7253-DB45-83E7-ADE40C20A309}">
+          <x14:formula1>
+            <xm:f>Metadata!$A$37:$A$41</xm:f>
+          </x14:formula1>
+          <xm:sqref>D32:D35</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C44D012F-7F42-4949-9DB6-889632F7F430}">
+          <x14:formula1>
+            <xm:f>Metadata!$A$33:$A$34</xm:f>
+          </x14:formula1>
+          <xm:sqref>C32</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FDBB9100-9189-9B46-AFA6-70F5744B59B1}">
+          <x14:formula1>
+            <xm:f>Metadata!$A$54:$A$56</xm:f>
+          </x14:formula1>
+          <xm:sqref>D25:D28</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A6E746B8-928B-C04E-A63F-C483C8EE772E}">
+          <x14:formula1>
+            <xm:f>Metadata!$A$48:$A$50</xm:f>
+          </x14:formula1>
+          <xm:sqref>C25:C28</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F366491D-7FFD-9645-9B4C-C52BCD9C1C84}">
+          <x14:formula1>
+            <xm:f>Metadata!$A$7:$A$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>B7:F7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{80DCE53B-DE9B-F14C-B38F-B0E62DBA7E9F}">
+          <x14:formula1>
+            <xm:f>Metadata!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5:F5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B493EE89-A164-D94C-8D13-983AB7C87FB9}">
+          <x14:formula1>
+            <xm:f>Metadata!$A$43:$A$44</xm:f>
+          </x14:formula1>
+          <xm:sqref>C15:C21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0416D6B4-1A88-D14C-AF33-860A0B4C2ADE}">
+          <x14:formula1>
+            <xm:f>Metadata!$A$21:$A$23</xm:f>
+          </x14:formula1>
+          <xm:sqref>D10:F10</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45AE6A66-6571-D24D-A307-DF57ADB3F673}">
+  <sheetPr codeName="Sheet4">
+    <tabColor theme="9"/>
+  </sheetPr>
+  <dimension ref="A1:F43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="6" width="30.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="83" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="85"/>
+    </row>
+    <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="97"/>
+    </row>
+    <row r="3" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="99"/>
+    </row>
+    <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="98"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="99"/>
+    </row>
+    <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="99"/>
+    </row>
+    <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="98"/>
+      <c r="C6" s="98"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="99"/>
+    </row>
+    <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="98"/>
+      <c r="C7" s="98"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="99"/>
+    </row>
+    <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="98"/>
+      <c r="C8" s="98"/>
+      <c r="D8" s="98"/>
+      <c r="E8" s="98"/>
+      <c r="F8" s="99"/>
+    </row>
+    <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="98"/>
+      <c r="C9" s="98"/>
+      <c r="D9" s="98"/>
+      <c r="E9" s="98"/>
+      <c r="F9" s="99"/>
+    </row>
+    <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="98"/>
+      <c r="C10" s="98"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="98"/>
+      <c r="F10" s="99"/>
+    </row>
+    <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="94"/>
+      <c r="C11" s="94"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="95"/>
+    </row>
+    <row r="12" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="105"/>
+      <c r="B12" s="106"/>
+      <c r="C12" s="106"/>
+      <c r="D12" s="106"/>
+      <c r="E12" s="106"/>
+      <c r="F12" s="107"/>
+    </row>
+    <row r="13" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="80" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="81"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="82"/>
+    </row>
+    <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="39"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="31"/>
+    </row>
+    <row r="16" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="39"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="31"/>
+    </row>
+    <row r="17" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="39"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="31"/>
+    </row>
+    <row r="18" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="39"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="31"/>
+    </row>
+    <row r="19" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="39"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="31"/>
+    </row>
+    <row r="20" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A20" s="39"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="31"/>
+    </row>
+    <row r="21" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="41"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="43"/>
+    </row>
+    <row r="22" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="105"/>
+      <c r="B22" s="106"/>
+      <c r="C22" s="106"/>
+      <c r="D22" s="106"/>
+      <c r="E22" s="106"/>
+      <c r="F22" s="107"/>
+    </row>
+    <row r="23" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="80" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="81"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="82"/>
+    </row>
+    <row r="24" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A24" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A25" s="39"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="31"/>
+    </row>
+    <row r="26" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A26" s="39"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="31"/>
+    </row>
+    <row r="27" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A27" s="39"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="31"/>
+    </row>
+    <row r="28" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A28" s="41"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="43"/>
+    </row>
+    <row r="29" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="105"/>
+      <c r="B29" s="106"/>
+      <c r="C29" s="106"/>
+      <c r="D29" s="106"/>
+      <c r="E29" s="106"/>
+      <c r="F29" s="107"/>
+    </row>
+    <row r="30" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="80" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="81"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="81"/>
+      <c r="F30" s="82"/>
+    </row>
+    <row r="31" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A31" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="96" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="96"/>
+      <c r="F31" s="97"/>
+    </row>
+    <row r="32" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A32" s="39"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="98"/>
+      <c r="E32" s="98"/>
+      <c r="F32" s="99"/>
+    </row>
+    <row r="33" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A33" s="39"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="98"/>
+      <c r="E33" s="98"/>
+      <c r="F33" s="99"/>
+    </row>
+    <row r="34" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A34" s="39"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="98"/>
+      <c r="E34" s="98"/>
+      <c r="F34" s="99"/>
+    </row>
+    <row r="35" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A35" s="41"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="94"/>
+      <c r="E35" s="94"/>
+      <c r="F35" s="95"/>
+    </row>
+    <row r="36" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="102"/>
+      <c r="B36" s="103"/>
+      <c r="C36" s="103"/>
+      <c r="D36" s="103"/>
+      <c r="E36" s="103"/>
+      <c r="F36" s="104"/>
+    </row>
+    <row r="37" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="80" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="81"/>
+      <c r="C37" s="81"/>
+      <c r="D37" s="81"/>
+      <c r="E37" s="81"/>
+      <c r="F37" s="82"/>
+    </row>
+    <row r="38" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="100"/>
+      <c r="B38" s="96"/>
+      <c r="C38" s="96"/>
+      <c r="D38" s="96"/>
+      <c r="E38" s="96"/>
+      <c r="F38" s="97"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="108"/>
+      <c r="B39" s="98"/>
+      <c r="C39" s="98"/>
+      <c r="D39" s="98"/>
+      <c r="E39" s="98"/>
+      <c r="F39" s="99"/>
+    </row>
+    <row r="40" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="105"/>
+      <c r="B40" s="106"/>
+      <c r="C40" s="106"/>
+      <c r="D40" s="106"/>
+      <c r="E40" s="106"/>
+      <c r="F40" s="107"/>
+    </row>
+    <row r="41" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="80" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="81"/>
+      <c r="C41" s="81"/>
+      <c r="D41" s="81"/>
+      <c r="E41" s="81"/>
+      <c r="F41" s="82"/>
+    </row>
+    <row r="42" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="100"/>
+      <c r="B42" s="96"/>
+      <c r="C42" s="96"/>
+      <c r="D42" s="96"/>
+      <c r="E42" s="96"/>
+      <c r="F42" s="97"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="101"/>
+      <c r="B43" s="94"/>
+      <c r="C43" s="94"/>
+      <c r="D43" s="94"/>
+      <c r="E43" s="94"/>
+      <c r="F43" s="95"/>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A38:F39"/>
+    <mergeCell ref="A42:F43"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A41:F41"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A13:F13"/>
@@ -8579,20 +10207,7 @@
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:F10"/>
-    <mergeCell ref="A42:F43"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A41:F41"/>
     <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A38:F39"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Colocar percentagem_x000a_" sqref="B10:C10" xr:uid="{C44B2955-AB0E-5E4A-9201-AF72D21AA99A}"/>
@@ -8659,7 +10274,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F56D591A-F277-D248-BC6E-ABCB9483D3AC}">
   <sheetPr codeName="Sheet5">
     <tabColor rgb="FFFF0000"/>
@@ -8885,7 +10500,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B34CF0A5-BCFD-6C4D-BD6A-52FE7B6EF76F}">
   <sheetPr codeName="Sheet6">
     <tabColor theme="6"/>

</xml_diff>

<commit_message>
docs warehouse customer emoployee saved
</commit_message>
<xml_diff>
--- a/docs/documentacao.xlsx
+++ b/docs/documentacao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micaelmbp/Documents/ENG-2022/TAAD/GlobalTech_ETL/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832CAC64-A47C-BE49-A3F4-9149CBCDF043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31F2C8A-689B-1143-BFAA-77DB3FBF64A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="3" xr2:uid="{1C0ABE59-C842-1448-8BFE-1E96A6C9A910}"/>
   </bookViews>
@@ -392,7 +392,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
@@ -880,11 +881,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1176,8 +1178,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -7260,7 +7272,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7866,9 +7878,9 @@
       <c r="A6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="90"/>
+      <c r="B6" s="109"/>
+      <c r="C6" s="110"/>
+      <c r="D6" s="111"/>
       <c r="E6" s="91" t="s">
         <v>58</v>
       </c>
@@ -8306,7 +8318,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:G5"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8775,7 +8787,7 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
DFM cancellation fact saved
</commit_message>
<xml_diff>
--- a/docs/documentacao.xlsx
+++ b/docs/documentacao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micaelmbp/Documents/ENG-2022/TAAD/GlobalTech_ETL/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A2CAE7-64E8-4445-9043-601ECE6103E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2842680-1515-5746-A03D-9E3101EB8A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="3" xr2:uid="{1C0ABE59-C842-1448-8BFE-1E96A6C9A910}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="116">
   <si>
     <t>Caracterização do Data Mart</t>
   </si>
@@ -386,6 +386,9 @@
   </si>
   <si>
     <t>Clientes que realizam as encomendas</t>
+  </si>
+  <si>
+    <t>1§</t>
   </si>
 </sst>
 </file>
@@ -8318,7 +8321,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8442,7 +8445,9 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
@@ -8754,7 +8759,7 @@
           <x14:formula1>
             <xm:f>Metadata!$A$27:$A$29</xm:f>
           </x14:formula1>
-          <xm:sqref>D10:D17</xm:sqref>
+          <xm:sqref>D11:D17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D1F5CADB-A877-C54F-BE54-46C783F98C6B}">
           <x14:formula1>

</xml_diff>

<commit_message>
all dims ready on ssis
</commit_message>
<xml_diff>
--- a/docs/documentacao.xlsx
+++ b/docs/documentacao.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaobraganca/Desktop/ParallelsShared/GlobalTech_ETL/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C648E047-66E3-754F-B41A-64ED30190002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC0A335-27E0-7745-9D6B-8CA459D1A4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8320" yWindow="2220" windowWidth="36460" windowHeight="22500" activeTab="3" xr2:uid="{1C0ABE59-C842-1448-8BFE-1E96A6C9A910}"/>
+    <workbookView xWindow="8320" yWindow="2220" windowWidth="36460" windowHeight="22500" activeTab="2" xr2:uid="{1C0ABE59-C842-1448-8BFE-1E96A6C9A910}"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz de decisão" sheetId="1" r:id="rId1"/>
@@ -1496,57 +1496,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1580,6 +1529,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1587,6 +1587,51 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1602,51 +1647,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7770,152 +7770,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="99"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="82"/>
     </row>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="122" t="s">
         <v>216</v>
       </c>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="108"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="123"/>
     </row>
     <row r="3" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="97" t="s">
         <v>202</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="79"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="98"/>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="97" t="s">
         <v>162</v>
       </c>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="79"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="98"/>
     </row>
     <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="78" t="s">
+      <c r="B5" s="97" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="79"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="98"/>
     </row>
     <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="97" t="s">
         <v>203</v>
       </c>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="79"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="98"/>
     </row>
     <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="79"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="97"/>
+      <c r="F7" s="98"/>
     </row>
     <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="97" t="s">
         <v>163</v>
       </c>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="79"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="98"/>
     </row>
     <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="79"/>
+      <c r="B9" s="97"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="98"/>
     </row>
     <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="109">
+      <c r="B10" s="124">
         <v>0.3</v>
       </c>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78" t="s">
+      <c r="C10" s="97"/>
+      <c r="D10" s="97" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="78"/>
-      <c r="F10" s="79"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="98"/>
     </row>
     <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="105" t="s">
+      <c r="B11" s="120" t="s">
         <v>164</v>
       </c>
-      <c r="C11" s="105"/>
-      <c r="D11" s="105"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="106"/>
+      <c r="C11" s="120"/>
+      <c r="D11" s="120"/>
+      <c r="E11" s="120"/>
+      <c r="F11" s="121"/>
     </row>
     <row r="12" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="113"/>
-      <c r="B12" s="114"/>
-      <c r="C12" s="114"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="114"/>
-      <c r="F12" s="115"/>
+      <c r="A12" s="111"/>
+      <c r="B12" s="112"/>
+      <c r="C12" s="112"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="112"/>
+      <c r="F12" s="113"/>
     </row>
     <row r="13" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="85" t="s">
+      <c r="A13" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="87"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="90"/>
     </row>
     <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
@@ -8081,14 +8081,14 @@
     </row>
     <row r="23" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="85" t="s">
+      <c r="A24" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="86"/>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="87"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="89"/>
+      <c r="F24" s="90"/>
     </row>
     <row r="25" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="39" t="s">
@@ -8147,22 +8147,22 @@
       <c r="F29" s="43"/>
     </row>
     <row r="30" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="113"/>
-      <c r="B30" s="114"/>
-      <c r="C30" s="114"/>
-      <c r="D30" s="114"/>
-      <c r="E30" s="114"/>
-      <c r="F30" s="115"/>
+      <c r="A30" s="111"/>
+      <c r="B30" s="112"/>
+      <c r="C30" s="112"/>
+      <c r="D30" s="112"/>
+      <c r="E30" s="112"/>
+      <c r="F30" s="113"/>
     </row>
     <row r="31" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="85" t="s">
+      <c r="A31" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="86"/>
-      <c r="C31" s="86"/>
-      <c r="D31" s="86"/>
-      <c r="E31" s="86"/>
-      <c r="F31" s="87"/>
+      <c r="B31" s="89"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="89"/>
+      <c r="E31" s="89"/>
+      <c r="F31" s="90"/>
     </row>
     <row r="32" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="39" t="s">
@@ -8174,114 +8174,130 @@
       <c r="C32" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="116" t="s">
+      <c r="D32" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="116"/>
-      <c r="F32" s="117"/>
+      <c r="E32" s="106"/>
+      <c r="F32" s="107"/>
     </row>
     <row r="33" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="39"/>
       <c r="B33" s="40"/>
       <c r="C33" s="40"/>
-      <c r="D33" s="118"/>
-      <c r="E33" s="118"/>
-      <c r="F33" s="119"/>
+      <c r="D33" s="109"/>
+      <c r="E33" s="109"/>
+      <c r="F33" s="110"/>
     </row>
     <row r="34" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="39"/>
       <c r="B34" s="40"/>
       <c r="C34" s="40"/>
-      <c r="D34" s="118"/>
-      <c r="E34" s="118"/>
-      <c r="F34" s="119"/>
+      <c r="D34" s="109"/>
+      <c r="E34" s="109"/>
+      <c r="F34" s="110"/>
     </row>
     <row r="35" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="39"/>
       <c r="B35" s="40"/>
       <c r="C35" s="40"/>
-      <c r="D35" s="118"/>
-      <c r="E35" s="118"/>
-      <c r="F35" s="119"/>
+      <c r="D35" s="109"/>
+      <c r="E35" s="109"/>
+      <c r="F35" s="110"/>
     </row>
     <row r="36" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="41"/>
       <c r="B36" s="42"/>
       <c r="C36" s="42"/>
-      <c r="D36" s="120"/>
-      <c r="E36" s="120"/>
-      <c r="F36" s="121"/>
+      <c r="D36" s="115"/>
+      <c r="E36" s="115"/>
+      <c r="F36" s="116"/>
     </row>
     <row r="37" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="110"/>
-      <c r="B37" s="111"/>
-      <c r="C37" s="111"/>
-      <c r="D37" s="111"/>
-      <c r="E37" s="111"/>
-      <c r="F37" s="112"/>
+      <c r="A37" s="117"/>
+      <c r="B37" s="118"/>
+      <c r="C37" s="118"/>
+      <c r="D37" s="118"/>
+      <c r="E37" s="118"/>
+      <c r="F37" s="119"/>
     </row>
     <row r="38" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="85" t="s">
+      <c r="A38" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="B38" s="86"/>
-      <c r="C38" s="86"/>
-      <c r="D38" s="86"/>
-      <c r="E38" s="86"/>
-      <c r="F38" s="87"/>
+      <c r="B38" s="89"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="89"/>
+      <c r="E38" s="89"/>
+      <c r="F38" s="90"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="122"/>
-      <c r="B39" s="116"/>
-      <c r="C39" s="116"/>
-      <c r="D39" s="116"/>
-      <c r="E39" s="116"/>
-      <c r="F39" s="117"/>
+      <c r="A39" s="105"/>
+      <c r="B39" s="106"/>
+      <c r="C39" s="106"/>
+      <c r="D39" s="106"/>
+      <c r="E39" s="106"/>
+      <c r="F39" s="107"/>
     </row>
     <row r="40" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="123"/>
-      <c r="B40" s="118"/>
-      <c r="C40" s="118"/>
-      <c r="D40" s="118"/>
-      <c r="E40" s="118"/>
-      <c r="F40" s="119"/>
+      <c r="A40" s="108"/>
+      <c r="B40" s="109"/>
+      <c r="C40" s="109"/>
+      <c r="D40" s="109"/>
+      <c r="E40" s="109"/>
+      <c r="F40" s="110"/>
     </row>
     <row r="41" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="113"/>
-      <c r="B41" s="114"/>
-      <c r="C41" s="114"/>
-      <c r="D41" s="114"/>
-      <c r="E41" s="114"/>
-      <c r="F41" s="115"/>
+      <c r="A41" s="111"/>
+      <c r="B41" s="112"/>
+      <c r="C41" s="112"/>
+      <c r="D41" s="112"/>
+      <c r="E41" s="112"/>
+      <c r="F41" s="113"/>
     </row>
     <row r="42" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="85" t="s">
+      <c r="A42" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="86"/>
-      <c r="C42" s="86"/>
-      <c r="D42" s="86"/>
-      <c r="E42" s="86"/>
-      <c r="F42" s="87"/>
+      <c r="B42" s="89"/>
+      <c r="C42" s="89"/>
+      <c r="D42" s="89"/>
+      <c r="E42" s="89"/>
+      <c r="F42" s="90"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="122"/>
-      <c r="B43" s="116"/>
-      <c r="C43" s="116"/>
-      <c r="D43" s="116"/>
-      <c r="E43" s="116"/>
-      <c r="F43" s="117"/>
+      <c r="A43" s="105"/>
+      <c r="B43" s="106"/>
+      <c r="C43" s="106"/>
+      <c r="D43" s="106"/>
+      <c r="E43" s="106"/>
+      <c r="F43" s="107"/>
     </row>
     <row r="44" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="124"/>
-      <c r="B44" s="120"/>
-      <c r="C44" s="120"/>
-      <c r="D44" s="120"/>
-      <c r="E44" s="120"/>
-      <c r="F44" s="121"/>
+      <c r="A44" s="114"/>
+      <c r="B44" s="115"/>
+      <c r="C44" s="115"/>
+      <c r="D44" s="115"/>
+      <c r="E44" s="115"/>
+      <c r="F44" s="116"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="A39:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A43:F44"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B2:F2"/>
@@ -8294,22 +8310,6 @@
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:F10"/>
-    <mergeCell ref="A37:F37"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="A38:F38"/>
-    <mergeCell ref="A39:F40"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A43:F44"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Colocar percentagem_x000a_" sqref="B10:C10" xr:uid="{2B355D78-2274-AF4C-B934-68ADBC7FB191}"/>
@@ -8764,7 +8764,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G2"/>
+      <selection activeCell="F10" sqref="F10:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8776,95 +8776,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="99"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="82"/>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="83" t="s">
         <v>209</v>
       </c>
       <c r="C2" s="68"/>
       <c r="D2" s="68"/>
       <c r="E2" s="68"/>
       <c r="F2" s="68"/>
-      <c r="G2" s="101"/>
+      <c r="G2" s="84"/>
     </row>
     <row r="3" spans="1:7" ht="46" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="85" t="s">
         <v>88</v>
       </c>
       <c r="C3" s="69"/>
       <c r="D3" s="69"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
-      <c r="G3" s="81"/>
+      <c r="G3" s="86"/>
     </row>
     <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="85" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="69"/>
       <c r="D4" s="69"/>
       <c r="E4" s="69"/>
       <c r="F4" s="69"/>
-      <c r="G4" s="81"/>
+      <c r="G4" s="86"/>
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="85" t="s">
         <v>87</v>
       </c>
       <c r="C5" s="69"/>
       <c r="D5" s="69"/>
       <c r="E5" s="69"/>
       <c r="F5" s="69"/>
-      <c r="G5" s="81"/>
+      <c r="G5" s="86"/>
     </row>
     <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="91"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="94" t="s">
+      <c r="B6" s="74"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="95"/>
-      <c r="G6" s="96"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="79"/>
     </row>
     <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="35"/>
       <c r="G7" s="33"/>
     </row>
     <row r="8" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="85" t="s">
+      <c r="A8" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="86"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="87"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="90"/>
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
@@ -9053,7 +9053,7 @@
       <c r="G18" s="37"/>
     </row>
     <row r="19" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A19" s="88" t="s">
+      <c r="A19" s="91" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="63"/>
@@ -9073,57 +9073,57 @@
       <c r="C20" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="89" t="s">
+      <c r="D20" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="89"/>
-      <c r="F20" s="89"/>
-      <c r="G20" s="89"/>
+      <c r="E20" s="92"/>
+      <c r="F20" s="92"/>
+      <c r="G20" s="92"/>
     </row>
     <row r="21" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="90"/>
-      <c r="E21" s="90"/>
-      <c r="F21" s="90"/>
-      <c r="G21" s="90"/>
+      <c r="D21" s="93"/>
+      <c r="E21" s="93"/>
+      <c r="F21" s="93"/>
+      <c r="G21" s="93"/>
     </row>
     <row r="22" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="90"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="90"/>
-      <c r="G22" s="90"/>
+      <c r="D22" s="93"/>
+      <c r="E22" s="93"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="93"/>
     </row>
     <row r="23" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="90"/>
-      <c r="E23" s="90"/>
-      <c r="F23" s="90"/>
-      <c r="G23" s="90"/>
+      <c r="D23" s="93"/>
+      <c r="E23" s="93"/>
+      <c r="F23" s="93"/>
+      <c r="G23" s="93"/>
     </row>
     <row r="24" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="90"/>
-      <c r="E24" s="90"/>
-      <c r="F24" s="90"/>
-      <c r="G24" s="90"/>
+      <c r="D24" s="93"/>
+      <c r="E24" s="93"/>
+      <c r="F24" s="93"/>
+      <c r="G24" s="93"/>
     </row>
     <row r="25" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="90"/>
-      <c r="E25" s="90"/>
-      <c r="F25" s="90"/>
-      <c r="G25" s="90"/>
+      <c r="D25" s="93"/>
+      <c r="E25" s="93"/>
+      <c r="F25" s="93"/>
+      <c r="G25" s="93"/>
     </row>
     <row r="26" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
@@ -9133,7 +9133,7 @@
       <c r="G26" s="33"/>
     </row>
     <row r="27" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A27" s="88" t="s">
+      <c r="A27" s="91" t="s">
         <v>29</v>
       </c>
       <c r="B27" s="63"/>
@@ -9150,13 +9150,13 @@
       <c r="B28" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="89" t="s">
+      <c r="C28" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="89"/>
-      <c r="E28" s="89"/>
-      <c r="F28" s="89"/>
-      <c r="G28" s="89"/>
+      <c r="D28" s="92"/>
+      <c r="E28" s="92"/>
+      <c r="F28" s="92"/>
+      <c r="G28" s="92"/>
     </row>
     <row r="29" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -9165,42 +9165,42 @@
       <c r="B29" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="74" t="s">
+      <c r="C29" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="87"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
     </row>
     <row r="30" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2</v>
       </c>
       <c r="B30" s="1"/>
-      <c r="C30" s="74" t="s">
+      <c r="C30" s="87" t="s">
         <v>112</v>
       </c>
-      <c r="D30" s="74"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
+      <c r="D30" s="87"/>
+      <c r="E30" s="87"/>
+      <c r="F30" s="87"/>
+      <c r="G30" s="87"/>
     </row>
     <row r="31" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="74"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="74"/>
+      <c r="C31" s="87"/>
+      <c r="D31" s="87"/>
+      <c r="E31" s="87"/>
+      <c r="F31" s="87"/>
+      <c r="G31" s="87"/>
     </row>
     <row r="32" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="G32" s="33"/>
     </row>
     <row r="33" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="75" t="s">
+      <c r="A33" s="94" t="s">
         <v>22</v>
       </c>
       <c r="B33" s="71"/>
@@ -9208,28 +9208,28 @@
       <c r="D33" s="71"/>
       <c r="E33" s="71"/>
       <c r="F33" s="71"/>
-      <c r="G33" s="76"/>
+      <c r="G33" s="95"/>
     </row>
     <row r="34" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="77"/>
-      <c r="B34" s="78"/>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="79"/>
+      <c r="A34" s="96"/>
+      <c r="B34" s="97"/>
+      <c r="C34" s="97"/>
+      <c r="D34" s="97"/>
+      <c r="E34" s="97"/>
+      <c r="F34" s="97"/>
+      <c r="G34" s="98"/>
     </row>
     <row r="35" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="77"/>
-      <c r="B35" s="78"/>
-      <c r="C35" s="78"/>
-      <c r="D35" s="78"/>
-      <c r="E35" s="78"/>
-      <c r="F35" s="78"/>
-      <c r="G35" s="79"/>
+      <c r="A35" s="96"/>
+      <c r="B35" s="97"/>
+      <c r="C35" s="97"/>
+      <c r="D35" s="97"/>
+      <c r="E35" s="97"/>
+      <c r="F35" s="97"/>
+      <c r="G35" s="98"/>
     </row>
     <row r="36" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="75" t="s">
+      <c r="A36" s="94" t="s">
         <v>10</v>
       </c>
       <c r="B36" s="71"/>
@@ -9237,35 +9237,33 @@
       <c r="D36" s="71"/>
       <c r="E36" s="71"/>
       <c r="F36" s="71"/>
-      <c r="G36" s="76"/>
+      <c r="G36" s="95"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="80"/>
+      <c r="A37" s="85"/>
       <c r="B37" s="69"/>
       <c r="C37" s="69"/>
       <c r="D37" s="69"/>
       <c r="E37" s="69"/>
       <c r="F37" s="69"/>
-      <c r="G37" s="81"/>
+      <c r="G37" s="86"/>
     </row>
     <row r="38" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="82"/>
-      <c r="B38" s="83"/>
-      <c r="C38" s="83"/>
-      <c r="D38" s="83"/>
-      <c r="E38" s="83"/>
-      <c r="F38" s="83"/>
-      <c r="G38" s="84"/>
+      <c r="A38" s="99"/>
+      <c r="B38" s="100"/>
+      <c r="C38" s="100"/>
+      <c r="D38" s="100"/>
+      <c r="E38" s="100"/>
+      <c r="F38" s="100"/>
+      <c r="G38" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A34:G35"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A37:G38"/>
     <mergeCell ref="C30:G30"/>
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="A19:G19"/>
@@ -9278,11 +9276,13 @@
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="C28:G28"/>
     <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="A34:G35"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A37:G38"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Exemplo:_x000a_id -&gt; nome -&gt; categoria -&gt; ALL" sqref="C29:C32" xr:uid="{386320E1-7050-C749-9143-6F7D856CB823}"/>
@@ -9340,8 +9340,8 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:F13"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9351,67 +9351,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="99"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="82"/>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="83" t="s">
         <v>210</v>
       </c>
       <c r="C2" s="68"/>
       <c r="D2" s="68"/>
       <c r="E2" s="68"/>
       <c r="F2" s="68"/>
-      <c r="G2" s="101"/>
+      <c r="G2" s="84"/>
     </row>
     <row r="3" spans="1:7" ht="46" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="85" t="s">
         <v>100</v>
       </c>
       <c r="C3" s="69"/>
       <c r="D3" s="69"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
-      <c r="G3" s="81"/>
+      <c r="G3" s="86"/>
     </row>
     <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="85" t="s">
         <v>53</v>
       </c>
       <c r="C4" s="69"/>
       <c r="D4" s="69"/>
       <c r="E4" s="69"/>
       <c r="F4" s="69"/>
-      <c r="G4" s="81"/>
+      <c r="G4" s="86"/>
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="85" t="s">
         <v>99</v>
       </c>
       <c r="C5" s="69"/>
       <c r="D5" s="69"/>
       <c r="E5" s="69"/>
       <c r="F5" s="69"/>
-      <c r="G5" s="81"/>
+      <c r="G5" s="86"/>
     </row>
     <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
@@ -9420,26 +9420,26 @@
       <c r="B6" s="102"/>
       <c r="C6" s="103"/>
       <c r="D6" s="104"/>
-      <c r="E6" s="94" t="s">
+      <c r="E6" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="95"/>
-      <c r="G6" s="96"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="79"/>
     </row>
     <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="35"/>
       <c r="G7" s="33"/>
     </row>
     <row r="8" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="85" t="s">
+      <c r="A8" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="86"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="87"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="90"/>
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
@@ -9540,7 +9540,7 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G13" s="1">
         <v>1</v>
@@ -9595,7 +9595,7 @@
       <c r="G17" s="37"/>
     </row>
     <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="88" t="s">
+      <c r="A18" s="91" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="63"/>
@@ -9615,57 +9615,57 @@
       <c r="C19" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="89" t="s">
+      <c r="D19" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="89"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="89"/>
+      <c r="E19" s="92"/>
+      <c r="F19" s="92"/>
+      <c r="G19" s="92"/>
     </row>
     <row r="20" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="90"/>
-      <c r="E20" s="90"/>
-      <c r="F20" s="90"/>
-      <c r="G20" s="90"/>
+      <c r="D20" s="93"/>
+      <c r="E20" s="93"/>
+      <c r="F20" s="93"/>
+      <c r="G20" s="93"/>
     </row>
     <row r="21" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="90"/>
-      <c r="E21" s="90"/>
-      <c r="F21" s="90"/>
-      <c r="G21" s="90"/>
+      <c r="D21" s="93"/>
+      <c r="E21" s="93"/>
+      <c r="F21" s="93"/>
+      <c r="G21" s="93"/>
     </row>
     <row r="22" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="90"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="90"/>
-      <c r="G22" s="90"/>
+      <c r="D22" s="93"/>
+      <c r="E22" s="93"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="93"/>
     </row>
     <row r="23" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="90"/>
-      <c r="E23" s="90"/>
-      <c r="F23" s="90"/>
-      <c r="G23" s="90"/>
+      <c r="D23" s="93"/>
+      <c r="E23" s="93"/>
+      <c r="F23" s="93"/>
+      <c r="G23" s="93"/>
     </row>
     <row r="24" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="90"/>
-      <c r="E24" s="90"/>
-      <c r="F24" s="90"/>
-      <c r="G24" s="90"/>
+      <c r="D24" s="93"/>
+      <c r="E24" s="93"/>
+      <c r="F24" s="93"/>
+      <c r="G24" s="93"/>
     </row>
     <row r="25" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="36"/>
@@ -9675,7 +9675,7 @@
       <c r="G25" s="33"/>
     </row>
     <row r="26" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A26" s="88" t="s">
+      <c r="A26" s="91" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="63"/>
@@ -9692,47 +9692,47 @@
       <c r="B27" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="89" t="s">
+      <c r="C27" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="89"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="89"/>
+      <c r="D27" s="92"/>
+      <c r="E27" s="92"/>
+      <c r="F27" s="92"/>
+      <c r="G27" s="92"/>
     </row>
     <row r="28" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
+      <c r="C28" s="87"/>
+      <c r="D28" s="87"/>
+      <c r="E28" s="87"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
     </row>
     <row r="29" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
+      <c r="C29" s="87"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="87"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
     </row>
     <row r="30" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
+      <c r="C30" s="87"/>
+      <c r="D30" s="87"/>
+      <c r="E30" s="87"/>
+      <c r="F30" s="87"/>
+      <c r="G30" s="87"/>
     </row>
     <row r="31" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="G31" s="33"/>
     </row>
     <row r="32" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="75" t="s">
+      <c r="A32" s="94" t="s">
         <v>22</v>
       </c>
       <c r="B32" s="71"/>
@@ -9740,28 +9740,28 @@
       <c r="D32" s="71"/>
       <c r="E32" s="71"/>
       <c r="F32" s="71"/>
-      <c r="G32" s="76"/>
+      <c r="G32" s="95"/>
     </row>
     <row r="33" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="77"/>
-      <c r="B33" s="78"/>
-      <c r="C33" s="78"/>
-      <c r="D33" s="78"/>
-      <c r="E33" s="78"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="79"/>
+      <c r="A33" s="96"/>
+      <c r="B33" s="97"/>
+      <c r="C33" s="97"/>
+      <c r="D33" s="97"/>
+      <c r="E33" s="97"/>
+      <c r="F33" s="97"/>
+      <c r="G33" s="98"/>
     </row>
     <row r="34" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="77"/>
-      <c r="B34" s="78"/>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="79"/>
+      <c r="A34" s="96"/>
+      <c r="B34" s="97"/>
+      <c r="C34" s="97"/>
+      <c r="D34" s="97"/>
+      <c r="E34" s="97"/>
+      <c r="F34" s="97"/>
+      <c r="G34" s="98"/>
     </row>
     <row r="35" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="75" t="s">
+      <c r="A35" s="94" t="s">
         <v>10</v>
       </c>
       <c r="B35" s="71"/>
@@ -9769,33 +9769,35 @@
       <c r="D35" s="71"/>
       <c r="E35" s="71"/>
       <c r="F35" s="71"/>
-      <c r="G35" s="76"/>
+      <c r="G35" s="95"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="80"/>
+      <c r="A36" s="85"/>
       <c r="B36" s="69"/>
       <c r="C36" s="69"/>
       <c r="D36" s="69"/>
       <c r="E36" s="69"/>
       <c r="F36" s="69"/>
-      <c r="G36" s="81"/>
+      <c r="G36" s="86"/>
     </row>
     <row r="37" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="82"/>
-      <c r="B37" s="83"/>
-      <c r="C37" s="83"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="83"/>
-      <c r="F37" s="83"/>
-      <c r="G37" s="84"/>
+      <c r="A37" s="99"/>
+      <c r="B37" s="100"/>
+      <c r="C37" s="100"/>
+      <c r="D37" s="100"/>
+      <c r="E37" s="100"/>
+      <c r="F37" s="100"/>
+      <c r="G37" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A33:G34"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A36:G37"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="A18:G18"/>
@@ -9808,13 +9810,11 @@
     <mergeCell ref="A26:G26"/>
     <mergeCell ref="C27:G27"/>
     <mergeCell ref="C28:G28"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A33:G34"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A36:G37"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Colocar percentagem" sqref="B6" xr:uid="{F51EFD33-359E-334A-A51E-A657A56E6972}">
@@ -9872,7 +9872,7 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -9884,95 +9884,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="99"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="82"/>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="83" t="s">
         <v>211</v>
       </c>
       <c r="C2" s="68"/>
       <c r="D2" s="68"/>
       <c r="E2" s="68"/>
       <c r="F2" s="68"/>
-      <c r="G2" s="101"/>
+      <c r="G2" s="84"/>
     </row>
     <row r="3" spans="1:7" ht="46" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="85" t="s">
         <v>148</v>
       </c>
       <c r="C3" s="69"/>
       <c r="D3" s="69"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
-      <c r="G3" s="81"/>
+      <c r="G3" s="86"/>
     </row>
     <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="85" t="s">
         <v>53</v>
       </c>
       <c r="C4" s="69"/>
       <c r="D4" s="69"/>
       <c r="E4" s="69"/>
       <c r="F4" s="69"/>
-      <c r="G4" s="81"/>
+      <c r="G4" s="86"/>
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="85" t="s">
         <v>110</v>
       </c>
       <c r="C5" s="69"/>
       <c r="D5" s="69"/>
       <c r="E5" s="69"/>
       <c r="F5" s="69"/>
-      <c r="G5" s="81"/>
+      <c r="G5" s="86"/>
     </row>
     <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="91"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="94" t="s">
+      <c r="B6" s="74"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="95"/>
-      <c r="G6" s="96"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="79"/>
     </row>
     <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="35"/>
       <c r="G7" s="33"/>
     </row>
     <row r="8" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="85" t="s">
+      <c r="A8" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="86"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="87"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="90"/>
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
@@ -10128,7 +10128,7 @@
       <c r="G17" s="37"/>
     </row>
     <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="88"/>
+      <c r="A18" s="91"/>
       <c r="B18" s="63"/>
       <c r="C18" s="63"/>
       <c r="D18" s="63"/>
@@ -10146,57 +10146,57 @@
       <c r="C19" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="89" t="s">
+      <c r="D19" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="89"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="89"/>
+      <c r="E19" s="92"/>
+      <c r="F19" s="92"/>
+      <c r="G19" s="92"/>
     </row>
     <row r="20" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="90"/>
-      <c r="E20" s="90"/>
-      <c r="F20" s="90"/>
-      <c r="G20" s="90"/>
+      <c r="D20" s="93"/>
+      <c r="E20" s="93"/>
+      <c r="F20" s="93"/>
+      <c r="G20" s="93"/>
     </row>
     <row r="21" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="90"/>
-      <c r="E21" s="90"/>
-      <c r="F21" s="90"/>
-      <c r="G21" s="90"/>
+      <c r="D21" s="93"/>
+      <c r="E21" s="93"/>
+      <c r="F21" s="93"/>
+      <c r="G21" s="93"/>
     </row>
     <row r="22" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="90"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="90"/>
-      <c r="G22" s="90"/>
+      <c r="D22" s="93"/>
+      <c r="E22" s="93"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="93"/>
     </row>
     <row r="23" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="90"/>
-      <c r="E23" s="90"/>
-      <c r="F23" s="90"/>
-      <c r="G23" s="90"/>
+      <c r="D23" s="93"/>
+      <c r="E23" s="93"/>
+      <c r="F23" s="93"/>
+      <c r="G23" s="93"/>
     </row>
     <row r="24" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="90"/>
-      <c r="E24" s="90"/>
-      <c r="F24" s="90"/>
-      <c r="G24" s="90"/>
+      <c r="D24" s="93"/>
+      <c r="E24" s="93"/>
+      <c r="F24" s="93"/>
+      <c r="G24" s="93"/>
     </row>
     <row r="25" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="36"/>
@@ -10206,7 +10206,7 @@
       <c r="G25" s="33"/>
     </row>
     <row r="26" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A26" s="88" t="s">
+      <c r="A26" s="91" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="63"/>
@@ -10223,47 +10223,47 @@
       <c r="B27" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="89" t="s">
+      <c r="C27" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="89"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="89"/>
+      <c r="D27" s="92"/>
+      <c r="E27" s="92"/>
+      <c r="F27" s="92"/>
+      <c r="G27" s="92"/>
     </row>
     <row r="28" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
+      <c r="C28" s="87"/>
+      <c r="D28" s="87"/>
+      <c r="E28" s="87"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
     </row>
     <row r="29" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
+      <c r="C29" s="87"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="87"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
     </row>
     <row r="30" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
+      <c r="C30" s="87"/>
+      <c r="D30" s="87"/>
+      <c r="E30" s="87"/>
+      <c r="F30" s="87"/>
+      <c r="G30" s="87"/>
     </row>
     <row r="31" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="G31" s="33"/>
     </row>
     <row r="32" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="75" t="s">
+      <c r="A32" s="94" t="s">
         <v>22</v>
       </c>
       <c r="B32" s="71"/>
@@ -10271,28 +10271,28 @@
       <c r="D32" s="71"/>
       <c r="E32" s="71"/>
       <c r="F32" s="71"/>
-      <c r="G32" s="76"/>
+      <c r="G32" s="95"/>
     </row>
     <row r="33" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="77"/>
-      <c r="B33" s="78"/>
-      <c r="C33" s="78"/>
-      <c r="D33" s="78"/>
-      <c r="E33" s="78"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="79"/>
+      <c r="A33" s="96"/>
+      <c r="B33" s="97"/>
+      <c r="C33" s="97"/>
+      <c r="D33" s="97"/>
+      <c r="E33" s="97"/>
+      <c r="F33" s="97"/>
+      <c r="G33" s="98"/>
     </row>
     <row r="34" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="77"/>
-      <c r="B34" s="78"/>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="79"/>
+      <c r="A34" s="96"/>
+      <c r="B34" s="97"/>
+      <c r="C34" s="97"/>
+      <c r="D34" s="97"/>
+      <c r="E34" s="97"/>
+      <c r="F34" s="97"/>
+      <c r="G34" s="98"/>
     </row>
     <row r="35" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="75" t="s">
+      <c r="A35" s="94" t="s">
         <v>10</v>
       </c>
       <c r="B35" s="71"/>
@@ -10300,36 +10300,28 @@
       <c r="D35" s="71"/>
       <c r="E35" s="71"/>
       <c r="F35" s="71"/>
-      <c r="G35" s="76"/>
+      <c r="G35" s="95"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="80"/>
+      <c r="A36" s="85"/>
       <c r="B36" s="69"/>
       <c r="C36" s="69"/>
       <c r="D36" s="69"/>
       <c r="E36" s="69"/>
       <c r="F36" s="69"/>
-      <c r="G36" s="81"/>
+      <c r="G36" s="86"/>
     </row>
     <row r="37" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="82"/>
-      <c r="B37" s="83"/>
-      <c r="C37" s="83"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="83"/>
-      <c r="F37" s="83"/>
-      <c r="G37" s="84"/>
+      <c r="A37" s="99"/>
+      <c r="B37" s="100"/>
+      <c r="C37" s="100"/>
+      <c r="D37" s="100"/>
+      <c r="E37" s="100"/>
+      <c r="F37" s="100"/>
+      <c r="G37" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="D23:G23"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="D20:G20"/>
@@ -10346,6 +10338,14 @@
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D23:G23"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Colocar percentagem" sqref="B6" xr:uid="{C5DD908A-3688-A14E-B89F-E074FAFCDF99}">
@@ -10415,95 +10415,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="99"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="82"/>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="83" t="s">
         <v>212</v>
       </c>
       <c r="C2" s="68"/>
       <c r="D2" s="68"/>
       <c r="E2" s="68"/>
       <c r="F2" s="68"/>
-      <c r="G2" s="101"/>
+      <c r="G2" s="84"/>
     </row>
     <row r="3" spans="1:7" ht="46" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="85" t="s">
         <v>124</v>
       </c>
       <c r="C3" s="69"/>
       <c r="D3" s="69"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
-      <c r="G3" s="81"/>
+      <c r="G3" s="86"/>
     </row>
     <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="85" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="69"/>
       <c r="D4" s="69"/>
       <c r="E4" s="69"/>
       <c r="F4" s="69"/>
-      <c r="G4" s="81"/>
+      <c r="G4" s="86"/>
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="85" t="s">
         <v>113</v>
       </c>
       <c r="C5" s="69"/>
       <c r="D5" s="69"/>
       <c r="E5" s="69"/>
       <c r="F5" s="69"/>
-      <c r="G5" s="81"/>
+      <c r="G5" s="86"/>
     </row>
     <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="91"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="94" t="s">
+      <c r="B6" s="74"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="95"/>
-      <c r="G6" s="96"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="79"/>
     </row>
     <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="35"/>
       <c r="G7" s="33"/>
     </row>
     <row r="8" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="85" t="s">
+      <c r="A8" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="86"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="87"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="90"/>
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
@@ -10647,7 +10647,7 @@
       <c r="G17" s="37"/>
     </row>
     <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="88" t="s">
+      <c r="A18" s="91" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="63"/>
@@ -10667,57 +10667,57 @@
       <c r="C19" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="89" t="s">
+      <c r="D19" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="89"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="89"/>
+      <c r="E19" s="92"/>
+      <c r="F19" s="92"/>
+      <c r="G19" s="92"/>
     </row>
     <row r="20" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="90"/>
-      <c r="E20" s="90"/>
-      <c r="F20" s="90"/>
-      <c r="G20" s="90"/>
+      <c r="D20" s="93"/>
+      <c r="E20" s="93"/>
+      <c r="F20" s="93"/>
+      <c r="G20" s="93"/>
     </row>
     <row r="21" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="90"/>
-      <c r="E21" s="90"/>
-      <c r="F21" s="90"/>
-      <c r="G21" s="90"/>
+      <c r="D21" s="93"/>
+      <c r="E21" s="93"/>
+      <c r="F21" s="93"/>
+      <c r="G21" s="93"/>
     </row>
     <row r="22" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="90"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="90"/>
-      <c r="G22" s="90"/>
+      <c r="D22" s="93"/>
+      <c r="E22" s="93"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="93"/>
     </row>
     <row r="23" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="90"/>
-      <c r="E23" s="90"/>
-      <c r="F23" s="90"/>
-      <c r="G23" s="90"/>
+      <c r="D23" s="93"/>
+      <c r="E23" s="93"/>
+      <c r="F23" s="93"/>
+      <c r="G23" s="93"/>
     </row>
     <row r="24" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="90"/>
-      <c r="E24" s="90"/>
-      <c r="F24" s="90"/>
-      <c r="G24" s="90"/>
+      <c r="D24" s="93"/>
+      <c r="E24" s="93"/>
+      <c r="F24" s="93"/>
+      <c r="G24" s="93"/>
     </row>
     <row r="25" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="36"/>
@@ -10727,7 +10727,7 @@
       <c r="G25" s="33"/>
     </row>
     <row r="26" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A26" s="88" t="s">
+      <c r="A26" s="91" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="63"/>
@@ -10744,47 +10744,47 @@
       <c r="B27" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="89" t="s">
+      <c r="C27" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="89"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="89"/>
+      <c r="D27" s="92"/>
+      <c r="E27" s="92"/>
+      <c r="F27" s="92"/>
+      <c r="G27" s="92"/>
     </row>
     <row r="28" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
+      <c r="C28" s="87"/>
+      <c r="D28" s="87"/>
+      <c r="E28" s="87"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
     </row>
     <row r="29" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
+      <c r="C29" s="87"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="87"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
     </row>
     <row r="30" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
+      <c r="C30" s="87"/>
+      <c r="D30" s="87"/>
+      <c r="E30" s="87"/>
+      <c r="F30" s="87"/>
+      <c r="G30" s="87"/>
     </row>
     <row r="31" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="G31" s="33"/>
     </row>
     <row r="32" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="75" t="s">
+      <c r="A32" s="94" t="s">
         <v>22</v>
       </c>
       <c r="B32" s="71"/>
@@ -10792,28 +10792,28 @@
       <c r="D32" s="71"/>
       <c r="E32" s="71"/>
       <c r="F32" s="71"/>
-      <c r="G32" s="76"/>
+      <c r="G32" s="95"/>
     </row>
     <row r="33" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="77"/>
-      <c r="B33" s="78"/>
-      <c r="C33" s="78"/>
-      <c r="D33" s="78"/>
-      <c r="E33" s="78"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="79"/>
+      <c r="A33" s="96"/>
+      <c r="B33" s="97"/>
+      <c r="C33" s="97"/>
+      <c r="D33" s="97"/>
+      <c r="E33" s="97"/>
+      <c r="F33" s="97"/>
+      <c r="G33" s="98"/>
     </row>
     <row r="34" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="77"/>
-      <c r="B34" s="78"/>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="79"/>
+      <c r="A34" s="96"/>
+      <c r="B34" s="97"/>
+      <c r="C34" s="97"/>
+      <c r="D34" s="97"/>
+      <c r="E34" s="97"/>
+      <c r="F34" s="97"/>
+      <c r="G34" s="98"/>
     </row>
     <row r="35" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="75" t="s">
+      <c r="A35" s="94" t="s">
         <v>10</v>
       </c>
       <c r="B35" s="71"/>
@@ -10821,33 +10821,35 @@
       <c r="D35" s="71"/>
       <c r="E35" s="71"/>
       <c r="F35" s="71"/>
-      <c r="G35" s="76"/>
+      <c r="G35" s="95"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="80"/>
+      <c r="A36" s="85"/>
       <c r="B36" s="69"/>
       <c r="C36" s="69"/>
       <c r="D36" s="69"/>
       <c r="E36" s="69"/>
       <c r="F36" s="69"/>
-      <c r="G36" s="81"/>
+      <c r="G36" s="86"/>
     </row>
     <row r="37" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="82"/>
-      <c r="B37" s="83"/>
-      <c r="C37" s="83"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="83"/>
-      <c r="F37" s="83"/>
-      <c r="G37" s="84"/>
+      <c r="A37" s="99"/>
+      <c r="B37" s="100"/>
+      <c r="C37" s="100"/>
+      <c r="D37" s="100"/>
+      <c r="E37" s="100"/>
+      <c r="F37" s="100"/>
+      <c r="G37" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A33:G34"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A36:G37"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="A18:G18"/>
@@ -10860,13 +10862,11 @@
     <mergeCell ref="A26:G26"/>
     <mergeCell ref="C27:G27"/>
     <mergeCell ref="C28:G28"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A33:G34"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A36:G37"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Exemplo:_x000a_id -&gt; nome -&gt; categoria -&gt; ALL" sqref="C28:C31" xr:uid="{6749BA4D-A4C0-664A-8057-C07B807E371B}"/>
@@ -10936,95 +10936,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="99"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="82"/>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="83" t="s">
         <v>213</v>
       </c>
       <c r="C2" s="68"/>
       <c r="D2" s="68"/>
       <c r="E2" s="68"/>
       <c r="F2" s="68"/>
-      <c r="G2" s="101"/>
+      <c r="G2" s="84"/>
     </row>
     <row r="3" spans="1:7" ht="46" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="85" t="s">
         <v>149</v>
       </c>
       <c r="C3" s="69"/>
       <c r="D3" s="69"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
-      <c r="G3" s="81"/>
+      <c r="G3" s="86"/>
     </row>
     <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="85" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="69"/>
       <c r="D4" s="69"/>
       <c r="E4" s="69"/>
       <c r="F4" s="69"/>
-      <c r="G4" s="81"/>
+      <c r="G4" s="86"/>
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="85" t="s">
         <v>150</v>
       </c>
       <c r="C5" s="69"/>
       <c r="D5" s="69"/>
       <c r="E5" s="69"/>
       <c r="F5" s="69"/>
-      <c r="G5" s="81"/>
+      <c r="G5" s="86"/>
     </row>
     <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="91"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="94" t="s">
+      <c r="B6" s="74"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="95"/>
-      <c r="G6" s="96"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="79"/>
     </row>
     <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="35"/>
       <c r="G7" s="33"/>
     </row>
     <row r="8" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="85" t="s">
+      <c r="A8" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="86"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="87"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="90"/>
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
@@ -11204,7 +11204,7 @@
       <c r="G17" s="37"/>
     </row>
     <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="88" t="s">
+      <c r="A18" s="91" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="63"/>
@@ -11224,57 +11224,57 @@
       <c r="C19" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="89" t="s">
+      <c r="D19" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="89"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="89"/>
+      <c r="E19" s="92"/>
+      <c r="F19" s="92"/>
+      <c r="G19" s="92"/>
     </row>
     <row r="20" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="90"/>
-      <c r="E20" s="90"/>
-      <c r="F20" s="90"/>
-      <c r="G20" s="90"/>
+      <c r="D20" s="93"/>
+      <c r="E20" s="93"/>
+      <c r="F20" s="93"/>
+      <c r="G20" s="93"/>
     </row>
     <row r="21" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="90"/>
-      <c r="E21" s="90"/>
-      <c r="F21" s="90"/>
-      <c r="G21" s="90"/>
+      <c r="D21" s="93"/>
+      <c r="E21" s="93"/>
+      <c r="F21" s="93"/>
+      <c r="G21" s="93"/>
     </row>
     <row r="22" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="90"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="90"/>
-      <c r="G22" s="90"/>
+      <c r="D22" s="93"/>
+      <c r="E22" s="93"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="93"/>
     </row>
     <row r="23" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="90"/>
-      <c r="E23" s="90"/>
-      <c r="F23" s="90"/>
-      <c r="G23" s="90"/>
+      <c r="D23" s="93"/>
+      <c r="E23" s="93"/>
+      <c r="F23" s="93"/>
+      <c r="G23" s="93"/>
     </row>
     <row r="24" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="90"/>
-      <c r="E24" s="90"/>
-      <c r="F24" s="90"/>
-      <c r="G24" s="90"/>
+      <c r="D24" s="93"/>
+      <c r="E24" s="93"/>
+      <c r="F24" s="93"/>
+      <c r="G24" s="93"/>
     </row>
     <row r="25" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="36"/>
@@ -11284,7 +11284,7 @@
       <c r="G25" s="33"/>
     </row>
     <row r="26" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A26" s="88" t="s">
+      <c r="A26" s="91" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="63"/>
@@ -11301,51 +11301,51 @@
       <c r="B27" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="89" t="s">
+      <c r="C27" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="89"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="89"/>
+      <c r="D27" s="92"/>
+      <c r="E27" s="92"/>
+      <c r="F27" s="92"/>
+      <c r="G27" s="92"/>
     </row>
     <row r="28" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1</v>
       </c>
       <c r="B28" s="1"/>
-      <c r="C28" s="74" t="s">
+      <c r="C28" s="87" t="s">
         <v>160</v>
       </c>
-      <c r="D28" s="74"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
+      <c r="D28" s="87"/>
+      <c r="E28" s="87"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
     </row>
     <row r="29" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
+      <c r="C29" s="87"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="87"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
     </row>
     <row r="30" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
+      <c r="C30" s="87"/>
+      <c r="D30" s="87"/>
+      <c r="E30" s="87"/>
+      <c r="F30" s="87"/>
+      <c r="G30" s="87"/>
     </row>
     <row r="31" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="G31" s="33"/>
     </row>
     <row r="32" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="75" t="s">
+      <c r="A32" s="94" t="s">
         <v>22</v>
       </c>
       <c r="B32" s="71"/>
@@ -11353,28 +11353,28 @@
       <c r="D32" s="71"/>
       <c r="E32" s="71"/>
       <c r="F32" s="71"/>
-      <c r="G32" s="76"/>
+      <c r="G32" s="95"/>
     </row>
     <row r="33" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="77"/>
-      <c r="B33" s="78"/>
-      <c r="C33" s="78"/>
-      <c r="D33" s="78"/>
-      <c r="E33" s="78"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="79"/>
+      <c r="A33" s="96"/>
+      <c r="B33" s="97"/>
+      <c r="C33" s="97"/>
+      <c r="D33" s="97"/>
+      <c r="E33" s="97"/>
+      <c r="F33" s="97"/>
+      <c r="G33" s="98"/>
     </row>
     <row r="34" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="77"/>
-      <c r="B34" s="78"/>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="79"/>
+      <c r="A34" s="96"/>
+      <c r="B34" s="97"/>
+      <c r="C34" s="97"/>
+      <c r="D34" s="97"/>
+      <c r="E34" s="97"/>
+      <c r="F34" s="97"/>
+      <c r="G34" s="98"/>
     </row>
     <row r="35" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="75" t="s">
+      <c r="A35" s="94" t="s">
         <v>10</v>
       </c>
       <c r="B35" s="71"/>
@@ -11382,33 +11382,35 @@
       <c r="D35" s="71"/>
       <c r="E35" s="71"/>
       <c r="F35" s="71"/>
-      <c r="G35" s="76"/>
+      <c r="G35" s="95"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="80"/>
+      <c r="A36" s="85"/>
       <c r="B36" s="69"/>
       <c r="C36" s="69"/>
       <c r="D36" s="69"/>
       <c r="E36" s="69"/>
       <c r="F36" s="69"/>
-      <c r="G36" s="81"/>
+      <c r="G36" s="86"/>
     </row>
     <row r="37" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="82"/>
-      <c r="B37" s="83"/>
-      <c r="C37" s="83"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="83"/>
-      <c r="F37" s="83"/>
-      <c r="G37" s="84"/>
+      <c r="A37" s="99"/>
+      <c r="B37" s="100"/>
+      <c r="C37" s="100"/>
+      <c r="D37" s="100"/>
+      <c r="E37" s="100"/>
+      <c r="F37" s="100"/>
+      <c r="G37" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A33:G34"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A36:G37"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="A18:G18"/>
@@ -11421,13 +11423,11 @@
     <mergeCell ref="A26:G26"/>
     <mergeCell ref="C27:G27"/>
     <mergeCell ref="C28:G28"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A33:G34"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A36:G37"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Colocar percentagem" sqref="B6" xr:uid="{A66D20F0-0782-6944-BA9C-7489AA303243}">
@@ -11498,152 +11498,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="99"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="82"/>
     </row>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="107">
+      <c r="B2" s="122">
         <v>4</v>
       </c>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="108"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="123"/>
     </row>
     <row r="3" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="97" t="s">
         <v>161</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="79"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="98"/>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="97" t="s">
         <v>162</v>
       </c>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="79"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="98"/>
     </row>
     <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="78" t="s">
+      <c r="B5" s="97" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="79"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="98"/>
     </row>
     <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="97" t="s">
         <v>207</v>
       </c>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="79"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="98"/>
     </row>
     <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="79"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="97"/>
+      <c r="F7" s="98"/>
     </row>
     <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="97" t="s">
         <v>163</v>
       </c>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="79"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="98"/>
     </row>
     <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="79"/>
+      <c r="B9" s="97"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="98"/>
     </row>
     <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="109">
+      <c r="B10" s="124">
         <v>0.5</v>
       </c>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78" t="s">
+      <c r="C10" s="97"/>
+      <c r="D10" s="97" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="78"/>
-      <c r="F10" s="79"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="98"/>
     </row>
     <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="105" t="s">
+      <c r="B11" s="120" t="s">
         <v>164</v>
       </c>
-      <c r="C11" s="105"/>
-      <c r="D11" s="105"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="106"/>
+      <c r="C11" s="120"/>
+      <c r="D11" s="120"/>
+      <c r="E11" s="120"/>
+      <c r="F11" s="121"/>
     </row>
     <row r="12" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="113"/>
-      <c r="B12" s="114"/>
-      <c r="C12" s="114"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="114"/>
-      <c r="F12" s="115"/>
+      <c r="A12" s="111"/>
+      <c r="B12" s="112"/>
+      <c r="C12" s="112"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="112"/>
+      <c r="F12" s="113"/>
     </row>
     <row r="13" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="85" t="s">
+      <c r="A13" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="87"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="90"/>
     </row>
     <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
@@ -11810,22 +11810,22 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="113"/>
-      <c r="B23" s="114"/>
-      <c r="C23" s="114"/>
-      <c r="D23" s="114"/>
-      <c r="E23" s="114"/>
-      <c r="F23" s="115"/>
+      <c r="A23" s="111"/>
+      <c r="B23" s="112"/>
+      <c r="C23" s="112"/>
+      <c r="D23" s="112"/>
+      <c r="E23" s="112"/>
+      <c r="F23" s="113"/>
     </row>
     <row r="24" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="85" t="s">
+      <c r="A24" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="86"/>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="87"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="89"/>
+      <c r="F24" s="90"/>
     </row>
     <row r="25" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="39" t="s">
@@ -11937,22 +11937,22 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="113"/>
-      <c r="B31" s="114"/>
-      <c r="C31" s="114"/>
-      <c r="D31" s="114"/>
-      <c r="E31" s="114"/>
-      <c r="F31" s="115"/>
+      <c r="A31" s="111"/>
+      <c r="B31" s="112"/>
+      <c r="C31" s="112"/>
+      <c r="D31" s="112"/>
+      <c r="E31" s="112"/>
+      <c r="F31" s="113"/>
     </row>
     <row r="32" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="85" t="s">
+      <c r="A32" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="86"/>
-      <c r="C32" s="86"/>
-      <c r="D32" s="86"/>
-      <c r="E32" s="86"/>
-      <c r="F32" s="87"/>
+      <c r="B32" s="89"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="89"/>
+      <c r="E32" s="89"/>
+      <c r="F32" s="90"/>
     </row>
     <row r="33" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="39" t="s">
@@ -11964,119 +11964,126 @@
       <c r="C33" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="116" t="s">
+      <c r="D33" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="E33" s="116"/>
-      <c r="F33" s="117"/>
+      <c r="E33" s="106"/>
+      <c r="F33" s="107"/>
     </row>
     <row r="34" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="39"/>
       <c r="B34" s="40"/>
       <c r="C34" s="40"/>
-      <c r="D34" s="118"/>
-      <c r="E34" s="118"/>
-      <c r="F34" s="119"/>
+      <c r="D34" s="109"/>
+      <c r="E34" s="109"/>
+      <c r="F34" s="110"/>
     </row>
     <row r="35" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="39"/>
       <c r="B35" s="40"/>
       <c r="C35" s="40"/>
-      <c r="D35" s="118"/>
-      <c r="E35" s="118"/>
-      <c r="F35" s="119"/>
+      <c r="D35" s="109"/>
+      <c r="E35" s="109"/>
+      <c r="F35" s="110"/>
     </row>
     <row r="36" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="39"/>
       <c r="B36" s="40"/>
       <c r="C36" s="40"/>
-      <c r="D36" s="118"/>
-      <c r="E36" s="118"/>
-      <c r="F36" s="119"/>
+      <c r="D36" s="109"/>
+      <c r="E36" s="109"/>
+      <c r="F36" s="110"/>
     </row>
     <row r="37" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="41"/>
       <c r="B37" s="42"/>
       <c r="C37" s="42"/>
-      <c r="D37" s="120"/>
-      <c r="E37" s="120"/>
-      <c r="F37" s="121"/>
+      <c r="D37" s="115"/>
+      <c r="E37" s="115"/>
+      <c r="F37" s="116"/>
     </row>
     <row r="38" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="110"/>
-      <c r="B38" s="111"/>
-      <c r="C38" s="111"/>
-      <c r="D38" s="111"/>
-      <c r="E38" s="111"/>
-      <c r="F38" s="112"/>
+      <c r="A38" s="117"/>
+      <c r="B38" s="118"/>
+      <c r="C38" s="118"/>
+      <c r="D38" s="118"/>
+      <c r="E38" s="118"/>
+      <c r="F38" s="119"/>
     </row>
     <row r="39" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="85" t="s">
+      <c r="A39" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="86"/>
-      <c r="C39" s="86"/>
-      <c r="D39" s="86"/>
-      <c r="E39" s="86"/>
-      <c r="F39" s="87"/>
+      <c r="B39" s="89"/>
+      <c r="C39" s="89"/>
+      <c r="D39" s="89"/>
+      <c r="E39" s="89"/>
+      <c r="F39" s="90"/>
     </row>
     <row r="40" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="122"/>
-      <c r="B40" s="116"/>
-      <c r="C40" s="116"/>
-      <c r="D40" s="116"/>
-      <c r="E40" s="116"/>
-      <c r="F40" s="117"/>
+      <c r="A40" s="105"/>
+      <c r="B40" s="106"/>
+      <c r="C40" s="106"/>
+      <c r="D40" s="106"/>
+      <c r="E40" s="106"/>
+      <c r="F40" s="107"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="123"/>
-      <c r="B41" s="118"/>
-      <c r="C41" s="118"/>
-      <c r="D41" s="118"/>
-      <c r="E41" s="118"/>
-      <c r="F41" s="119"/>
+      <c r="A41" s="108"/>
+      <c r="B41" s="109"/>
+      <c r="C41" s="109"/>
+      <c r="D41" s="109"/>
+      <c r="E41" s="109"/>
+      <c r="F41" s="110"/>
     </row>
     <row r="42" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="113"/>
-      <c r="B42" s="114"/>
-      <c r="C42" s="114"/>
-      <c r="D42" s="114"/>
-      <c r="E42" s="114"/>
-      <c r="F42" s="115"/>
+      <c r="A42" s="111"/>
+      <c r="B42" s="112"/>
+      <c r="C42" s="112"/>
+      <c r="D42" s="112"/>
+      <c r="E42" s="112"/>
+      <c r="F42" s="113"/>
     </row>
     <row r="43" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="85" t="s">
+      <c r="A43" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="B43" s="86"/>
-      <c r="C43" s="86"/>
-      <c r="D43" s="86"/>
-      <c r="E43" s="86"/>
-      <c r="F43" s="87"/>
+      <c r="B43" s="89"/>
+      <c r="C43" s="89"/>
+      <c r="D43" s="89"/>
+      <c r="E43" s="89"/>
+      <c r="F43" s="90"/>
     </row>
     <row r="44" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="122"/>
-      <c r="B44" s="116"/>
-      <c r="C44" s="116"/>
-      <c r="D44" s="116"/>
-      <c r="E44" s="116"/>
-      <c r="F44" s="117"/>
+      <c r="A44" s="105"/>
+      <c r="B44" s="106"/>
+      <c r="C44" s="106"/>
+      <c r="D44" s="106"/>
+      <c r="E44" s="106"/>
+      <c r="F44" s="107"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="124"/>
-      <c r="B45" s="120"/>
-      <c r="C45" s="120"/>
-      <c r="D45" s="120"/>
-      <c r="E45" s="120"/>
-      <c r="F45" s="121"/>
+      <c r="A45" s="114"/>
+      <c r="B45" s="115"/>
+      <c r="C45" s="115"/>
+      <c r="D45" s="115"/>
+      <c r="E45" s="115"/>
+      <c r="F45" s="116"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A40:F41"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="A44:F45"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
     <mergeCell ref="A38:F38"/>
     <mergeCell ref="A12:F12"/>
     <mergeCell ref="A13:F13"/>
@@ -12089,18 +12096,11 @@
     <mergeCell ref="D35:F35"/>
     <mergeCell ref="D36:F36"/>
     <mergeCell ref="D37:F37"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A40:F41"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="A44:F45"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="5">
@@ -12189,152 +12189,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="99"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="82"/>
     </row>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="122" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="108"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="123"/>
     </row>
     <row r="3" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="97" t="s">
         <v>183</v>
       </c>
-      <c r="C3" s="118"/>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="119"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="110"/>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="97" t="s">
         <v>162</v>
       </c>
-      <c r="C4" s="118"/>
-      <c r="D4" s="118"/>
-      <c r="E4" s="118"/>
-      <c r="F4" s="119"/>
+      <c r="C4" s="109"/>
+      <c r="D4" s="109"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="110"/>
     </row>
     <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="78" t="s">
+      <c r="B5" s="97" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="118"/>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
-      <c r="F5" s="119"/>
+      <c r="C5" s="109"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="110"/>
     </row>
     <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="97" t="s">
         <v>204</v>
       </c>
-      <c r="C6" s="118"/>
-      <c r="D6" s="118"/>
-      <c r="E6" s="118"/>
-      <c r="F6" s="119"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="110"/>
     </row>
     <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="118"/>
-      <c r="D7" s="118"/>
-      <c r="E7" s="118"/>
-      <c r="F7" s="119"/>
+      <c r="C7" s="109"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="110"/>
     </row>
     <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="97" t="s">
         <v>163</v>
       </c>
-      <c r="C8" s="118"/>
-      <c r="D8" s="118"/>
-      <c r="E8" s="118"/>
-      <c r="F8" s="119"/>
+      <c r="C8" s="109"/>
+      <c r="D8" s="109"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="110"/>
     </row>
     <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="118"/>
-      <c r="C9" s="118"/>
-      <c r="D9" s="118"/>
-      <c r="E9" s="118"/>
-      <c r="F9" s="119"/>
+      <c r="B9" s="109"/>
+      <c r="C9" s="109"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="110"/>
     </row>
     <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="109">
+      <c r="B10" s="124">
         <v>0.7</v>
       </c>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78" t="s">
+      <c r="C10" s="97"/>
+      <c r="D10" s="97" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="78"/>
-      <c r="F10" s="79"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="98"/>
     </row>
     <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="105" t="s">
+      <c r="B11" s="120" t="s">
         <v>164</v>
       </c>
-      <c r="C11" s="120"/>
-      <c r="D11" s="120"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="121"/>
+      <c r="C11" s="115"/>
+      <c r="D11" s="115"/>
+      <c r="E11" s="115"/>
+      <c r="F11" s="116"/>
     </row>
     <row r="12" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="113"/>
-      <c r="B12" s="114"/>
-      <c r="C12" s="114"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="114"/>
-      <c r="F12" s="115"/>
+      <c r="A12" s="111"/>
+      <c r="B12" s="112"/>
+      <c r="C12" s="112"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="112"/>
+      <c r="F12" s="113"/>
     </row>
     <row r="13" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="85" t="s">
+      <c r="A13" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="87"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="90"/>
     </row>
     <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
@@ -12553,22 +12553,22 @@
       <c r="F26" s="55"/>
     </row>
     <row r="27" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="113"/>
-      <c r="B27" s="114"/>
-      <c r="C27" s="114"/>
-      <c r="D27" s="114"/>
-      <c r="E27" s="114"/>
-      <c r="F27" s="115"/>
+      <c r="A27" s="111"/>
+      <c r="B27" s="112"/>
+      <c r="C27" s="112"/>
+      <c r="D27" s="112"/>
+      <c r="E27" s="112"/>
+      <c r="F27" s="113"/>
     </row>
     <row r="28" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="85" t="s">
+      <c r="A28" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="86"/>
-      <c r="C28" s="86"/>
-      <c r="D28" s="86"/>
-      <c r="E28" s="86"/>
-      <c r="F28" s="87"/>
+      <c r="B28" s="89"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="89"/>
+      <c r="F28" s="90"/>
     </row>
     <row r="29" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="39" t="s">
@@ -12641,22 +12641,22 @@
       <c r="F33" s="43"/>
     </row>
     <row r="34" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="113"/>
-      <c r="B34" s="114"/>
-      <c r="C34" s="114"/>
-      <c r="D34" s="114"/>
-      <c r="E34" s="114"/>
-      <c r="F34" s="115"/>
+      <c r="A34" s="111"/>
+      <c r="B34" s="112"/>
+      <c r="C34" s="112"/>
+      <c r="D34" s="112"/>
+      <c r="E34" s="112"/>
+      <c r="F34" s="113"/>
     </row>
     <row r="35" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="85" t="s">
+      <c r="A35" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="B35" s="86"/>
-      <c r="C35" s="86"/>
-      <c r="D35" s="86"/>
-      <c r="E35" s="86"/>
-      <c r="F35" s="87"/>
+      <c r="B35" s="89"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="89"/>
+      <c r="E35" s="89"/>
+      <c r="F35" s="90"/>
     </row>
     <row r="36" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="39" t="s">
@@ -12668,127 +12668,114 @@
       <c r="C36" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="116" t="s">
+      <c r="D36" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="E36" s="116"/>
-      <c r="F36" s="117"/>
+      <c r="E36" s="106"/>
+      <c r="F36" s="107"/>
     </row>
     <row r="37" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="39"/>
       <c r="B37" s="40"/>
       <c r="C37" s="40"/>
-      <c r="D37" s="118"/>
-      <c r="E37" s="118"/>
-      <c r="F37" s="119"/>
+      <c r="D37" s="109"/>
+      <c r="E37" s="109"/>
+      <c r="F37" s="110"/>
     </row>
     <row r="38" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="39"/>
       <c r="B38" s="40"/>
       <c r="C38" s="40"/>
-      <c r="D38" s="118"/>
-      <c r="E38" s="118"/>
-      <c r="F38" s="119"/>
+      <c r="D38" s="109"/>
+      <c r="E38" s="109"/>
+      <c r="F38" s="110"/>
     </row>
     <row r="39" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="39"/>
       <c r="B39" s="40"/>
       <c r="C39" s="40"/>
-      <c r="D39" s="118"/>
-      <c r="E39" s="118"/>
-      <c r="F39" s="119"/>
+      <c r="D39" s="109"/>
+      <c r="E39" s="109"/>
+      <c r="F39" s="110"/>
     </row>
     <row r="40" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="41"/>
       <c r="B40" s="42"/>
       <c r="C40" s="42"/>
-      <c r="D40" s="120"/>
-      <c r="E40" s="120"/>
-      <c r="F40" s="121"/>
+      <c r="D40" s="115"/>
+      <c r="E40" s="115"/>
+      <c r="F40" s="116"/>
     </row>
     <row r="41" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="110"/>
-      <c r="B41" s="111"/>
-      <c r="C41" s="111"/>
-      <c r="D41" s="111"/>
-      <c r="E41" s="111"/>
-      <c r="F41" s="112"/>
+      <c r="A41" s="117"/>
+      <c r="B41" s="118"/>
+      <c r="C41" s="118"/>
+      <c r="D41" s="118"/>
+      <c r="E41" s="118"/>
+      <c r="F41" s="119"/>
     </row>
     <row r="42" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="85" t="s">
+      <c r="A42" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="86"/>
-      <c r="C42" s="86"/>
-      <c r="D42" s="86"/>
-      <c r="E42" s="86"/>
-      <c r="F42" s="87"/>
+      <c r="B42" s="89"/>
+      <c r="C42" s="89"/>
+      <c r="D42" s="89"/>
+      <c r="E42" s="89"/>
+      <c r="F42" s="90"/>
     </row>
     <row r="43" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="122"/>
-      <c r="B43" s="116"/>
-      <c r="C43" s="116"/>
-      <c r="D43" s="116"/>
-      <c r="E43" s="116"/>
-      <c r="F43" s="117"/>
+      <c r="A43" s="105"/>
+      <c r="B43" s="106"/>
+      <c r="C43" s="106"/>
+      <c r="D43" s="106"/>
+      <c r="E43" s="106"/>
+      <c r="F43" s="107"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="123"/>
-      <c r="B44" s="118"/>
-      <c r="C44" s="118"/>
-      <c r="D44" s="118"/>
-      <c r="E44" s="118"/>
-      <c r="F44" s="119"/>
+      <c r="A44" s="108"/>
+      <c r="B44" s="109"/>
+      <c r="C44" s="109"/>
+      <c r="D44" s="109"/>
+      <c r="E44" s="109"/>
+      <c r="F44" s="110"/>
     </row>
     <row r="45" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="113"/>
-      <c r="B45" s="114"/>
-      <c r="C45" s="114"/>
-      <c r="D45" s="114"/>
-      <c r="E45" s="114"/>
-      <c r="F45" s="115"/>
+      <c r="A45" s="111"/>
+      <c r="B45" s="112"/>
+      <c r="C45" s="112"/>
+      <c r="D45" s="112"/>
+      <c r="E45" s="112"/>
+      <c r="F45" s="113"/>
     </row>
     <row r="46" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="85" t="s">
+      <c r="A46" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="B46" s="86"/>
-      <c r="C46" s="86"/>
-      <c r="D46" s="86"/>
-      <c r="E46" s="86"/>
-      <c r="F46" s="87"/>
+      <c r="B46" s="89"/>
+      <c r="C46" s="89"/>
+      <c r="D46" s="89"/>
+      <c r="E46" s="89"/>
+      <c r="F46" s="90"/>
     </row>
     <row r="47" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="122"/>
-      <c r="B47" s="116"/>
-      <c r="C47" s="116"/>
-      <c r="D47" s="116"/>
-      <c r="E47" s="116"/>
-      <c r="F47" s="117"/>
+      <c r="A47" s="105"/>
+      <c r="B47" s="106"/>
+      <c r="C47" s="106"/>
+      <c r="D47" s="106"/>
+      <c r="E47" s="106"/>
+      <c r="F47" s="107"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="124"/>
-      <c r="B48" s="120"/>
-      <c r="C48" s="120"/>
-      <c r="D48" s="120"/>
-      <c r="E48" s="120"/>
-      <c r="F48" s="121"/>
+      <c r="A48" s="114"/>
+      <c r="B48" s="115"/>
+      <c r="C48" s="115"/>
+      <c r="D48" s="115"/>
+      <c r="E48" s="115"/>
+      <c r="F48" s="116"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="A43:F44"/>
-    <mergeCell ref="A47:F48"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A13:F13"/>
@@ -12805,6 +12792,19 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A43:F44"/>
+    <mergeCell ref="A47:F48"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Colocar percentagem_x000a_" sqref="B10:C10" xr:uid="{C44B2955-AB0E-5E4A-9201-AF72D21AA99A}"/>
@@ -12890,152 +12890,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="99"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="82"/>
     </row>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="122" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="108"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="123"/>
     </row>
     <row r="3" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="97" t="s">
         <v>179</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="79"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="98"/>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="97" t="s">
         <v>162</v>
       </c>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="79"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="98"/>
     </row>
     <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="78" t="s">
+      <c r="B5" s="97" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="79"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="98"/>
     </row>
     <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="97" t="s">
         <v>208</v>
       </c>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="79"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="98"/>
     </row>
     <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="79"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="97"/>
+      <c r="F7" s="98"/>
     </row>
     <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="97" t="s">
         <v>163</v>
       </c>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="79"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="98"/>
     </row>
     <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="79"/>
+      <c r="B9" s="97"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="98"/>
     </row>
     <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="109">
+      <c r="B10" s="124">
         <v>0.5</v>
       </c>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78" t="s">
+      <c r="C10" s="97"/>
+      <c r="D10" s="97" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="78"/>
-      <c r="F10" s="79"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="98"/>
     </row>
     <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="105" t="s">
+      <c r="B11" s="120" t="s">
         <v>164</v>
       </c>
-      <c r="C11" s="105"/>
-      <c r="D11" s="105"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="106"/>
+      <c r="C11" s="120"/>
+      <c r="D11" s="120"/>
+      <c r="E11" s="120"/>
+      <c r="F11" s="121"/>
     </row>
     <row r="12" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="113"/>
-      <c r="B12" s="114"/>
-      <c r="C12" s="114"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="114"/>
-      <c r="F12" s="115"/>
+      <c r="A12" s="111"/>
+      <c r="B12" s="112"/>
+      <c r="C12" s="112"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="112"/>
+      <c r="F12" s="113"/>
     </row>
     <row r="13" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="85" t="s">
+      <c r="A13" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="87"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="90"/>
     </row>
     <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
@@ -13166,22 +13166,22 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="113"/>
-      <c r="B21" s="114"/>
-      <c r="C21" s="114"/>
-      <c r="D21" s="114"/>
-      <c r="E21" s="114"/>
-      <c r="F21" s="115"/>
+      <c r="A21" s="111"/>
+      <c r="B21" s="112"/>
+      <c r="C21" s="112"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="112"/>
+      <c r="F21" s="113"/>
     </row>
     <row r="22" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="85" t="s">
+      <c r="A22" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="B22" s="86"/>
-      <c r="C22" s="86"/>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="87"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
+      <c r="E22" s="89"/>
+      <c r="F22" s="90"/>
     </row>
     <row r="23" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="39" t="s">
@@ -13255,22 +13255,22 @@
       <c r="F27" s="43"/>
     </row>
     <row r="28" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="113"/>
-      <c r="B28" s="114"/>
-      <c r="C28" s="114"/>
-      <c r="D28" s="114"/>
-      <c r="E28" s="114"/>
-      <c r="F28" s="115"/>
+      <c r="A28" s="111"/>
+      <c r="B28" s="112"/>
+      <c r="C28" s="112"/>
+      <c r="D28" s="112"/>
+      <c r="E28" s="112"/>
+      <c r="F28" s="113"/>
     </row>
     <row r="29" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="85" t="s">
+      <c r="A29" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="86"/>
-      <c r="C29" s="86"/>
-      <c r="D29" s="86"/>
-      <c r="E29" s="86"/>
-      <c r="F29" s="87"/>
+      <c r="B29" s="89"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="89"/>
+      <c r="E29" s="89"/>
+      <c r="F29" s="90"/>
     </row>
     <row r="30" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="39" t="s">
@@ -13282,114 +13282,131 @@
       <c r="C30" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="116" t="s">
+      <c r="D30" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="116"/>
-      <c r="F30" s="117"/>
+      <c r="E30" s="106"/>
+      <c r="F30" s="107"/>
     </row>
     <row r="31" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="39"/>
       <c r="B31" s="40"/>
       <c r="C31" s="40"/>
-      <c r="D31" s="118"/>
-      <c r="E31" s="118"/>
-      <c r="F31" s="119"/>
+      <c r="D31" s="109"/>
+      <c r="E31" s="109"/>
+      <c r="F31" s="110"/>
     </row>
     <row r="32" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="39"/>
       <c r="B32" s="40"/>
       <c r="C32" s="40"/>
-      <c r="D32" s="118"/>
-      <c r="E32" s="118"/>
-      <c r="F32" s="119"/>
+      <c r="D32" s="109"/>
+      <c r="E32" s="109"/>
+      <c r="F32" s="110"/>
     </row>
     <row r="33" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="39"/>
       <c r="B33" s="40"/>
       <c r="C33" s="40"/>
-      <c r="D33" s="118"/>
-      <c r="E33" s="118"/>
-      <c r="F33" s="119"/>
+      <c r="D33" s="109"/>
+      <c r="E33" s="109"/>
+      <c r="F33" s="110"/>
     </row>
     <row r="34" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="41"/>
       <c r="B34" s="42"/>
       <c r="C34" s="42"/>
-      <c r="D34" s="120"/>
-      <c r="E34" s="120"/>
-      <c r="F34" s="121"/>
+      <c r="D34" s="115"/>
+      <c r="E34" s="115"/>
+      <c r="F34" s="116"/>
     </row>
     <row r="35" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="110"/>
-      <c r="B35" s="111"/>
-      <c r="C35" s="111"/>
-      <c r="D35" s="111"/>
-      <c r="E35" s="111"/>
-      <c r="F35" s="112"/>
+      <c r="A35" s="117"/>
+      <c r="B35" s="118"/>
+      <c r="C35" s="118"/>
+      <c r="D35" s="118"/>
+      <c r="E35" s="118"/>
+      <c r="F35" s="119"/>
     </row>
     <row r="36" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="85" t="s">
+      <c r="A36" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="86"/>
-      <c r="C36" s="86"/>
-      <c r="D36" s="86"/>
-      <c r="E36" s="86"/>
-      <c r="F36" s="87"/>
+      <c r="B36" s="89"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="89"/>
+      <c r="E36" s="89"/>
+      <c r="F36" s="90"/>
     </row>
     <row r="37" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="122"/>
-      <c r="B37" s="116"/>
-      <c r="C37" s="116"/>
-      <c r="D37" s="116"/>
-      <c r="E37" s="116"/>
-      <c r="F37" s="117"/>
+      <c r="A37" s="105"/>
+      <c r="B37" s="106"/>
+      <c r="C37" s="106"/>
+      <c r="D37" s="106"/>
+      <c r="E37" s="106"/>
+      <c r="F37" s="107"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="123"/>
-      <c r="B38" s="118"/>
-      <c r="C38" s="118"/>
-      <c r="D38" s="118"/>
-      <c r="E38" s="118"/>
-      <c r="F38" s="119"/>
+      <c r="A38" s="108"/>
+      <c r="B38" s="109"/>
+      <c r="C38" s="109"/>
+      <c r="D38" s="109"/>
+      <c r="E38" s="109"/>
+      <c r="F38" s="110"/>
     </row>
     <row r="39" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="113"/>
-      <c r="B39" s="114"/>
-      <c r="C39" s="114"/>
-      <c r="D39" s="114"/>
-      <c r="E39" s="114"/>
-      <c r="F39" s="115"/>
+      <c r="A39" s="111"/>
+      <c r="B39" s="112"/>
+      <c r="C39" s="112"/>
+      <c r="D39" s="112"/>
+      <c r="E39" s="112"/>
+      <c r="F39" s="113"/>
     </row>
     <row r="40" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="85" t="s">
+      <c r="A40" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="86"/>
-      <c r="C40" s="86"/>
-      <c r="D40" s="86"/>
-      <c r="E40" s="86"/>
-      <c r="F40" s="87"/>
+      <c r="B40" s="89"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="89"/>
+      <c r="E40" s="89"/>
+      <c r="F40" s="90"/>
     </row>
     <row r="41" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="122"/>
-      <c r="B41" s="116"/>
-      <c r="C41" s="116"/>
-      <c r="D41" s="116"/>
-      <c r="E41" s="116"/>
-      <c r="F41" s="117"/>
+      <c r="A41" s="105"/>
+      <c r="B41" s="106"/>
+      <c r="C41" s="106"/>
+      <c r="D41" s="106"/>
+      <c r="E41" s="106"/>
+      <c r="F41" s="107"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="124"/>
-      <c r="B42" s="120"/>
-      <c r="C42" s="120"/>
-      <c r="D42" s="120"/>
-      <c r="E42" s="120"/>
-      <c r="F42" s="121"/>
+      <c r="A42" s="114"/>
+      <c r="B42" s="115"/>
+      <c r="C42" s="115"/>
+      <c r="D42" s="115"/>
+      <c r="E42" s="115"/>
+      <c r="F42" s="116"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A37:F38"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A41:F42"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B2:F2"/>
@@ -13402,23 +13419,6 @@
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:F10"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A37:F38"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A41:F42"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Colocar percentagem_x000a_" sqref="B10:C10" xr:uid="{8EDB03EC-30FB-484C-ACBE-DF33B9366718}"/>
@@ -13486,9 +13486,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13630,26 +13633,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30DE7E78-AB24-4BCB-A51F-77E5C10364A7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCF46D4-6C3F-4211-BBB9-5DE005064C3C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="6597237e-e321-437a-ab0e-fe3e3f709099"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13673,9 +13665,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCF46D4-6C3F-4211-BBB9-5DE005064C3C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30DE7E78-AB24-4BCB-A51F-77E5C10364A7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="6597237e-e321-437a-ab0e-fe3e3f709099"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>